<commit_message>
Update ICM to v4, add '96 consists
</commit_message>
<xml_diff>
--- a/historisch.xlsx
+++ b/historisch.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Code\quickdrive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E48A775-8BF7-475D-9498-85D13AFBD0E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6090527-5889-4B9A-92FD-A5B7D82B1EE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2625" windowWidth="21503" windowHeight="12975" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="675" yWindow="2055" windowWidth="21503" windowHeight="12975" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="86-87" sheetId="1" r:id="rId1"/>
@@ -5972,10 +5972,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8601,8 +8597,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{778DD009-53DD-426B-BBA7-ABCE73A49F39}">
   <dimension ref="A1:C77"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B41" sqref="A41:B44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -8625,34 +8621,37 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>106</v>
-      </c>
-      <c r="B2">
-        <v>360</v>
+        <v>89</v>
+      </c>
+      <c r="B2" t="s">
+        <v>90</v>
       </c>
       <c r="C2" t="s">
-        <v>157</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>95</v>
-      </c>
-      <c r="B3">
-        <v>800</v>
+        <v>92</v>
+      </c>
+      <c r="B3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C3" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>93</v>
       </c>
       <c r="B4">
-        <v>800</v>
+        <v>5400</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>95</v>
       </c>
       <c r="B5">
         <v>800</v>
@@ -8660,229 +8659,232 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>95</v>
       </c>
       <c r="B6">
-        <v>800</v>
+        <v>900</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>98</v>
       </c>
       <c r="B7">
-        <v>800</v>
+        <v>3100</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>121</v>
+        <v>98</v>
       </c>
       <c r="B8">
-        <v>800</v>
+        <v>3200</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>25</v>
+        <v>98</v>
       </c>
       <c r="B9">
-        <v>800</v>
+        <v>4000</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="B10">
-        <v>900</v>
+        <v>5300</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>36</v>
+        <v>98</v>
       </c>
       <c r="B11">
-        <v>900</v>
+        <v>5400</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>98</v>
       </c>
       <c r="B12">
-        <v>900</v>
+        <v>5900</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>18</v>
+        <v>98</v>
       </c>
       <c r="B13">
-        <v>900</v>
+        <v>9600</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B14">
-        <v>900</v>
+        <v>8200</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>121</v>
+        <v>13</v>
       </c>
       <c r="B15">
-        <v>900</v>
+        <v>8300</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="B16">
-        <v>900</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
+        <v>8600</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17">
+        <v>8700</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18">
+        <v>8800</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A19" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19">
+        <v>8900</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A20" t="s">
+        <v>156</v>
+      </c>
+      <c r="B20">
+        <v>6200</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A21" t="s">
+        <v>156</v>
+      </c>
+      <c r="B21">
+        <v>7700</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A22" t="s">
+        <v>106</v>
+      </c>
+      <c r="B22">
+        <v>360</v>
+      </c>
+      <c r="C22" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A23" t="s">
+        <v>106</v>
+      </c>
+      <c r="B23">
+        <v>1900</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A24" t="s">
         <v>36</v>
       </c>
-      <c r="B17">
-        <v>1500</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A18" t="s">
-        <v>109</v>
-      </c>
-      <c r="B18">
-        <v>1500</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A19" t="s">
-        <v>16</v>
-      </c>
-      <c r="B19">
-        <v>1500</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A20" t="s">
-        <v>19</v>
-      </c>
-      <c r="B20">
-        <v>1500</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A21" t="s">
-        <v>25</v>
-      </c>
-      <c r="B21">
-        <v>1600</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A22" t="s">
-        <v>36</v>
-      </c>
-      <c r="B22">
-        <v>1800</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A23" t="s">
-        <v>19</v>
-      </c>
-      <c r="B23">
-        <v>1800</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A24" t="s">
-        <v>106</v>
-      </c>
       <c r="B24">
-        <v>1900</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>36</v>
       </c>
       <c r="B25">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A26" t="s">
+        <v>36</v>
+      </c>
+      <c r="B26">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A27" t="s">
+        <v>36</v>
+      </c>
+      <c r="B27">
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A28" t="s">
+        <v>36</v>
+      </c>
+      <c r="B28">
         <v>1900</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A26" t="s">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A29" t="s">
+        <v>109</v>
+      </c>
+      <c r="B29">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A30" t="s">
         <v>111</v>
       </c>
-      <c r="B26">
+      <c r="B30">
         <v>3000</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A27" t="s">
-        <v>98</v>
-      </c>
-      <c r="B27">
-        <v>3100</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A28" t="s">
-        <v>20</v>
-      </c>
-      <c r="B28">
-        <v>3100</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A29" t="s">
-        <v>98</v>
-      </c>
-      <c r="B29">
-        <v>3200</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A30" t="s">
-        <v>20</v>
-      </c>
-      <c r="B30">
-        <v>3200</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
-        <v>11</v>
+        <v>111</v>
       </c>
       <c r="B31">
-        <v>3400</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.45">
+        <v>3600</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
+        <v>112</v>
+      </c>
+      <c r="C32" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A33" t="s">
         <v>7</v>
       </c>
-      <c r="B32">
+      <c r="B33">
         <v>3500</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A33" t="s">
-        <v>111</v>
-      </c>
-      <c r="B33">
-        <v>3600</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>7</v>
       </c>
@@ -8890,282 +8892,270 @@
         <v>3600</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
-        <v>9</v>
-      </c>
-      <c r="B35">
-        <v>3600</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.45">
+        <v>153</v>
+      </c>
+      <c r="C35" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
-        <v>146</v>
+        <v>17</v>
       </c>
       <c r="B36">
-        <v>3800</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.45">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
-        <v>98</v>
+        <v>17</v>
       </c>
       <c r="B37">
-        <v>4000</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.45">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
+        <v>18</v>
+      </c>
+      <c r="B38">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A39" t="s">
+        <v>18</v>
+      </c>
+      <c r="B39">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A40" t="s">
+        <v>16</v>
+      </c>
+      <c r="B40">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A41" t="s">
+        <v>19</v>
+      </c>
+      <c r="B41">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A42" t="s">
+        <v>19</v>
+      </c>
+      <c r="B42">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A43" t="s">
+        <v>19</v>
+      </c>
+      <c r="B43">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A44" t="s">
+        <v>19</v>
+      </c>
+      <c r="B44">
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A45" t="s">
         <v>20</v>
       </c>
-      <c r="B38">
-        <v>4000</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A39" t="s">
-        <v>98</v>
-      </c>
-      <c r="B39">
-        <v>5300</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A40" t="s">
-        <v>20</v>
-      </c>
-      <c r="B40">
-        <v>5300</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A41" t="s">
-        <v>93</v>
-      </c>
-      <c r="B41">
-        <v>5400</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A42" t="s">
-        <v>98</v>
-      </c>
-      <c r="B42">
-        <v>5400</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A43" t="s">
-        <v>20</v>
-      </c>
-      <c r="B43">
-        <v>5400</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A44" t="s">
-        <v>152</v>
-      </c>
-      <c r="B44">
-        <v>5400</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A45" t="s">
-        <v>98</v>
-      </c>
       <c r="B45">
-        <v>5900</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.45">
+        <v>3100</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
         <v>20</v>
       </c>
       <c r="B46">
-        <v>5900</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.45">
+        <v>3200</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
-        <v>156</v>
+        <v>20</v>
       </c>
       <c r="B47">
-        <v>6200</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.45">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="B48">
-        <v>7200</v>
+        <v>5300</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
-        <v>156</v>
+        <v>20</v>
       </c>
       <c r="B49">
-        <v>7700</v>
+        <v>5400</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="B50">
-        <v>7700</v>
+        <v>5900</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="B51">
-        <v>7800</v>
+        <v>9600</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
-        <v>10</v>
+        <v>152</v>
       </c>
       <c r="B52">
-        <v>7900</v>
+        <v>5400</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
-        <v>146</v>
-      </c>
-      <c r="B53">
-        <v>8000</v>
+        <v>47</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
-        <v>13</v>
-      </c>
-      <c r="B54">
-        <v>8200</v>
+        <v>120</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
-        <v>13</v>
+        <v>121</v>
       </c>
       <c r="B55">
-        <v>8300</v>
+        <v>800</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
-        <v>13</v>
+        <v>121</v>
       </c>
       <c r="B56">
-        <v>8600</v>
+        <v>900</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B57">
-        <v>8700</v>
+        <v>3600</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B58">
-        <v>8800</v>
+        <v>9700</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B59">
-        <v>8900</v>
+        <v>7200</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
-        <v>155</v>
+        <v>10</v>
       </c>
       <c r="B60">
-        <v>9300</v>
+        <v>7700</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
-        <v>155</v>
+        <v>10</v>
       </c>
       <c r="B61">
-        <v>9400</v>
+        <v>7800</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
-        <v>98</v>
+        <v>10</v>
       </c>
       <c r="B62">
-        <v>9600</v>
+        <v>7900</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="B63">
-        <v>9600</v>
+        <v>16600</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B64">
-        <v>9700</v>
+        <v>3400</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="B65">
-        <v>16600</v>
+        <v>800</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="B66">
-        <v>18900</v>
+        <v>900</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
-        <v>89</v>
-      </c>
-      <c r="B67" t="s">
-        <v>90</v>
-      </c>
-      <c r="C67" t="s">
-        <v>91</v>
+        <v>25</v>
+      </c>
+      <c r="B67">
+        <v>1600</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
-        <v>92</v>
-      </c>
-      <c r="B68" t="s">
-        <v>90</v>
-      </c>
-      <c r="C68" t="s">
-        <v>91</v>
+        <v>12</v>
+      </c>
+      <c r="B68">
+        <v>18900</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.45">
@@ -9181,44 +9171,50 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
-        <v>112</v>
+        <v>142</v>
       </c>
       <c r="C70" t="s">
-        <v>113</v>
+        <v>143</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A71" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="C71" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A72" t="s">
-        <v>47</v>
+        <v>146</v>
+      </c>
+      <c r="B72">
+        <v>3800</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
-        <v>120</v>
+        <v>146</v>
+      </c>
+      <c r="B73">
+        <v>8000</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A74" t="s">
-        <v>142</v>
-      </c>
-      <c r="C74" t="s">
-        <v>143</v>
+        <v>155</v>
+      </c>
+      <c r="B74">
+        <v>9300</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A75" t="s">
-        <v>144</v>
-      </c>
-      <c r="C75" t="s">
-        <v>145</v>
+        <v>155</v>
+      </c>
+      <c r="B75">
+        <v>9400</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.45">
@@ -9240,7 +9236,7 @@
   </sheetData>
   <autoFilter ref="A1:C76" xr:uid="{778DD009-53DD-426B-BBA7-ABCE73A49F39}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C77">
-      <sortCondition ref="B1:B76"/>
+      <sortCondition ref="A1:A76"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10115,7 +10111,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DB840A4-93DF-43F4-B9FF-1DFD0858F8C3}">
   <dimension ref="A1:H562"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A154" workbookViewId="0">
+    <sheetView topLeftCell="A154" workbookViewId="0">
       <selection activeCell="I163" sqref="I163"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Bugfixes, added scenario to git
</commit_message>
<xml_diff>
--- a/historisch.xlsx
+++ b/historisch.xlsx
@@ -8,23 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Code\quickdrive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7941EFD-9EAF-42E3-8D88-DD9D38A71DA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ACC668F-9205-4844-9981-7C2CCA9B13DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1275" yWindow="2280" windowWidth="21502" windowHeight="12975" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2850" yWindow="2093" windowWidth="15247" windowHeight="11647" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="86-87" sheetId="1" r:id="rId1"/>
-    <sheet name="95-96" sheetId="2" r:id="rId2"/>
-    <sheet name="96-97" sheetId="3" r:id="rId3"/>
-    <sheet name="Goederenwagens" sheetId="6" r:id="rId4"/>
-    <sheet name="D-Treinen" sheetId="7" r:id="rId5"/>
+    <sheet name="76-77" sheetId="9" r:id="rId1"/>
+    <sheet name="86-87" sheetId="1" r:id="rId2"/>
+    <sheet name="95-96" sheetId="2" r:id="rId3"/>
+    <sheet name="96-97" sheetId="3" r:id="rId4"/>
+    <sheet name="Goederenwagens" sheetId="6" r:id="rId5"/>
+    <sheet name="D-Treinen" sheetId="7" r:id="rId6"/>
+    <sheet name="Tijdlijn" sheetId="8" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'86-87'!$A$1:$D$115</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'95-96'!$A$1:$C$100</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'96-97'!$A$1:$C$101</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'D-Treinen'!$A$1:$H$562</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Goederenwagens!$A$1:$I$52</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'76-77'!$A$1:$D$138</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'86-87'!$A$1:$D$115</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'95-96'!$A$1:$C$100</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'96-97'!$A$1:$C$101</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'D-Treinen'!$A$1:$H$562</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Goederenwagens!$A$1:$I$52</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -4711,7 +4714,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2551" uniqueCount="379">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2689" uniqueCount="428">
   <si>
     <t>ICM (KLM, Martinair)</t>
   </si>
@@ -5848,6 +5851,153 @@
   </si>
   <si>
     <t>Grensverkeer Em</t>
+  </si>
+  <si>
+    <t>Arriva</t>
+  </si>
+  <si>
+    <t>Connexxion</t>
+  </si>
+  <si>
+    <t>Veolia</t>
+  </si>
+  <si>
+    <t>DE</t>
+  </si>
+  <si>
+    <t>419 (Groen)</t>
+  </si>
+  <si>
+    <t>Groen</t>
+  </si>
+  <si>
+    <t>Geel</t>
+  </si>
+  <si>
+    <t>SpitsPendel</t>
+  </si>
+  <si>
+    <t>NachtSprinter</t>
+  </si>
+  <si>
+    <t>StrandSprinter</t>
+  </si>
+  <si>
+    <t>CityPendel</t>
+  </si>
+  <si>
+    <t>Vlaflip</t>
+  </si>
+  <si>
+    <t>Plan V?</t>
+  </si>
+  <si>
+    <t>Pec</t>
+  </si>
+  <si>
+    <t>682, 683</t>
+  </si>
+  <si>
+    <t>4679, 4684</t>
+  </si>
+  <si>
+    <t>1589 Rtd-Ehv</t>
+  </si>
+  <si>
+    <t>783 (2x Pec, Rtd-Mpl-Lw/Gn); 782 Gn-Rtd, 774 Lw-Asd</t>
+  </si>
+  <si>
+    <t>4374, 4385, 4330 Zo</t>
+  </si>
+  <si>
+    <t>Mat'46</t>
+  </si>
+  <si>
+    <t>DE1/2?</t>
+  </si>
+  <si>
+    <t>Mat'54</t>
+  </si>
+  <si>
+    <t>Mat'57 Benelux</t>
+  </si>
+  <si>
+    <t>Plan U?</t>
+  </si>
+  <si>
+    <t>Stalen D?</t>
+  </si>
+  <si>
+    <t>Plan D</t>
+  </si>
+  <si>
+    <t>2244, 2247</t>
+  </si>
+  <si>
+    <t>Plan K</t>
+  </si>
+  <si>
+    <t>Plan N</t>
+  </si>
+  <si>
+    <t>Slaaprijtuigen T2s</t>
+  </si>
+  <si>
+    <t>D1313, D1312</t>
+  </si>
+  <si>
+    <t>NS 1100?</t>
+  </si>
+  <si>
+    <t>NS 1000</t>
+  </si>
+  <si>
+    <t>Goederen</t>
+  </si>
+  <si>
+    <t>NS 1500</t>
+  </si>
+  <si>
+    <t>TEE7</t>
+  </si>
+  <si>
+    <t>D2241</t>
+  </si>
+  <si>
+    <t>+ Plan C, E of L, of Gs</t>
+  </si>
+  <si>
+    <t>oa Ertstreinen Awhv-Em</t>
+  </si>
+  <si>
+    <t>D236: DSB B, NS T2s, DB AB, DB AB, DB AB, NS D</t>
+  </si>
+  <si>
+    <t>D234, D237, 230. D216?</t>
+  </si>
+  <si>
+    <t>oa VAM Dt/Sdm-Bkh</t>
+  </si>
+  <si>
+    <t>NS 1300?</t>
+  </si>
+  <si>
+    <t>NS 1200?</t>
+  </si>
+  <si>
+    <t>Allen beneden de rivieren toegestaan. Oa VAM trein Rsw</t>
+  </si>
+  <si>
+    <t>D-trein Parijs</t>
+  </si>
+  <si>
+    <t>NS 1500?</t>
+  </si>
+  <si>
+    <t>Plan K?</t>
+  </si>
+  <si>
+    <t>Plan N?</t>
   </si>
 </sst>
 </file>
@@ -5920,7 +6070,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -5945,6 +6095,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -5959,7 +6121,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -5979,6 +6141,31 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -6259,11 +6446,1077 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1F2546F-C082-477C-B976-7FC2D49CF31C}">
+  <dimension ref="A1:D142"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="16.6640625" customWidth="1"/>
+    <col min="2" max="2" width="14.796875" customWidth="1"/>
+    <col min="3" max="3" width="23.59765625" style="20" customWidth="1"/>
+    <col min="4" max="4" width="18.59765625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>401</v>
+      </c>
+      <c r="B2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A3" s="18" t="s">
+        <v>392</v>
+      </c>
+      <c r="B3" s="18">
+        <v>100</v>
+      </c>
+      <c r="C3" s="21">
+        <v>189</v>
+      </c>
+      <c r="D3" s="2"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A4" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="18">
+        <v>200</v>
+      </c>
+      <c r="C4" s="21" t="s">
+        <v>418</v>
+      </c>
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>413</v>
+      </c>
+      <c r="B5">
+        <v>200</v>
+      </c>
+      <c r="C5" s="20" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B6">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>392</v>
+      </c>
+      <c r="B7">
+        <v>600</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B8">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>392</v>
+      </c>
+      <c r="B9">
+        <v>700</v>
+      </c>
+      <c r="C9" s="20" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B10">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>398</v>
+      </c>
+      <c r="B11">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>410</v>
+      </c>
+      <c r="B12">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A16" t="s">
+        <v>410</v>
+      </c>
+      <c r="B16">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A19" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A20" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A21" t="s">
+        <v>403</v>
+      </c>
+      <c r="B21">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A22" t="s">
+        <v>408</v>
+      </c>
+      <c r="B22">
+        <v>1300</v>
+      </c>
+      <c r="C22" s="20" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A23" t="s">
+        <v>427</v>
+      </c>
+      <c r="B23">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A24" t="s">
+        <v>426</v>
+      </c>
+      <c r="B24">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A25" t="s">
+        <v>425</v>
+      </c>
+      <c r="B25">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A26" t="s">
+        <v>392</v>
+      </c>
+      <c r="B26">
+        <v>1500</v>
+      </c>
+      <c r="C26" s="20" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A27" t="s">
+        <v>422</v>
+      </c>
+      <c r="B27">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A28" t="s">
+        <v>404</v>
+      </c>
+      <c r="B28">
+        <v>1600</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A29" t="s">
+        <v>24</v>
+      </c>
+      <c r="B29">
+        <v>1600</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A30" t="s">
+        <v>25</v>
+      </c>
+      <c r="B30">
+        <v>1600</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A31" t="s">
+        <v>400</v>
+      </c>
+      <c r="B31">
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B32">
+        <v>2030</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A33" t="s">
+        <v>398</v>
+      </c>
+      <c r="B33">
+        <v>2100</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A34" t="s">
+        <v>401</v>
+      </c>
+      <c r="B34">
+        <v>2100</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A35" t="s">
+        <v>392</v>
+      </c>
+      <c r="B35">
+        <v>2100</v>
+      </c>
+      <c r="C35" s="20">
+        <v>2187</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A36" t="s">
+        <v>413</v>
+      </c>
+      <c r="B36">
+        <v>2200</v>
+      </c>
+      <c r="C36" s="20" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A37" t="s">
+        <v>404</v>
+      </c>
+      <c r="B37">
+        <v>2200</v>
+      </c>
+      <c r="C37" s="20" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A38" t="s">
+        <v>421</v>
+      </c>
+      <c r="B38">
+        <v>2300</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A39" t="s">
+        <v>422</v>
+      </c>
+      <c r="B39">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A40" t="s">
+        <v>413</v>
+      </c>
+      <c r="B40">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A41" t="s">
+        <v>406</v>
+      </c>
+      <c r="B41">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A42" t="s">
+        <v>407</v>
+      </c>
+      <c r="B42">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A43" t="s">
+        <v>403</v>
+      </c>
+      <c r="B43">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A44" t="s">
+        <v>398</v>
+      </c>
+      <c r="B44">
+        <v>2600</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A45" t="s">
+        <v>398</v>
+      </c>
+      <c r="B45">
+        <v>2700</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A46" t="s">
+        <v>391</v>
+      </c>
+      <c r="B46">
+        <v>2800</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B47">
+        <v>2900</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A48" t="s">
+        <v>398</v>
+      </c>
+      <c r="B48">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B49">
+        <v>3100</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B50">
+        <v>3200</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B51">
+        <v>3300</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B52">
+        <v>3500</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B53">
+        <v>3600</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B54">
+        <v>3730</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B55">
+        <v>3770</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B56">
+        <v>3900</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A57" t="s">
+        <v>398</v>
+      </c>
+      <c r="B57">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A58" t="s">
+        <v>398</v>
+      </c>
+      <c r="B58">
+        <v>4100</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A59" t="s">
+        <v>12</v>
+      </c>
+      <c r="B59">
+        <v>4100</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A60" t="s">
+        <v>391</v>
+      </c>
+      <c r="B60">
+        <v>4200</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A61" t="s">
+        <v>12</v>
+      </c>
+      <c r="B61">
+        <v>4200</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A62" t="s">
+        <v>392</v>
+      </c>
+      <c r="B62">
+        <v>4300</v>
+      </c>
+      <c r="C62" s="20" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A63" t="s">
+        <v>24</v>
+      </c>
+      <c r="B63">
+        <v>4300</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A64" t="s">
+        <v>398</v>
+      </c>
+      <c r="B64">
+        <v>4500</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A65" t="s">
+        <v>391</v>
+      </c>
+      <c r="B65">
+        <v>4500</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A66" t="s">
+        <v>392</v>
+      </c>
+      <c r="B66">
+        <v>4600</v>
+      </c>
+      <c r="C66" s="20" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A67" t="s">
+        <v>24</v>
+      </c>
+      <c r="B67">
+        <v>4600</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A68" t="s">
+        <v>398</v>
+      </c>
+      <c r="B68">
+        <v>4700</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B69">
+        <v>4800</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B70">
+        <v>4900</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A71" t="s">
+        <v>398</v>
+      </c>
+      <c r="B71">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B72">
+        <v>5100</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A73" t="s">
+        <v>398</v>
+      </c>
+      <c r="B73">
+        <v>5200</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B74">
+        <v>5300</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A75" t="s">
+        <v>401</v>
+      </c>
+      <c r="B75">
+        <v>5400</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B76">
+        <v>5500</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B77">
+        <v>5600</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B78">
+        <v>5700</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B79">
+        <v>5800</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B80">
+        <v>6100</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A81" t="s">
+        <v>402</v>
+      </c>
+      <c r="B81">
+        <v>6200</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B82">
+        <v>6300</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B83">
+        <v>6400</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A84" t="s">
+        <v>47</v>
+      </c>
+      <c r="B84">
+        <v>6500</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A85" t="s">
+        <v>45</v>
+      </c>
+      <c r="B85">
+        <v>6500</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A86" t="s">
+        <v>24</v>
+      </c>
+      <c r="B86">
+        <v>6500</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B87">
+        <v>6600</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B88">
+        <v>6700</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A89" t="s">
+        <v>398</v>
+      </c>
+      <c r="B89">
+        <v>6800</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B90">
+        <v>6900</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A91" t="s">
+        <v>400</v>
+      </c>
+      <c r="B91">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A92" t="s">
+        <v>10</v>
+      </c>
+      <c r="B92">
+        <v>7100</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A93" t="s">
+        <v>399</v>
+      </c>
+      <c r="B93">
+        <v>7200</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A94" t="s">
+        <v>391</v>
+      </c>
+      <c r="B94">
+        <v>7300</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A95" t="s">
+        <v>398</v>
+      </c>
+      <c r="B95">
+        <v>7400</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B96">
+        <v>7500</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B97">
+        <v>7600</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A98" t="s">
+        <v>402</v>
+      </c>
+      <c r="B98">
+        <v>7700</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A99" t="s">
+        <v>47</v>
+      </c>
+      <c r="B99">
+        <v>7700</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B100">
+        <v>7800</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B101">
+        <v>7900</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A102" t="s">
+        <v>402</v>
+      </c>
+      <c r="B102">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B103">
+        <v>8100</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B104">
+        <v>8200</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B105">
+        <v>8300</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B106">
+        <v>8400</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B107">
+        <v>8500</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A108" t="s">
+        <v>402</v>
+      </c>
+      <c r="B108">
+        <v>8600</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A109" t="s">
+        <v>1</v>
+      </c>
+      <c r="B109">
+        <v>8700</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A110" t="s">
+        <v>1</v>
+      </c>
+      <c r="B110">
+        <v>8800</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B111">
+        <v>8900</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B112">
+        <v>9600</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A113" t="s">
+        <v>391</v>
+      </c>
+      <c r="B113">
+        <v>9700</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B114">
+        <v>9800</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B115">
+        <v>9900</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B116">
+        <v>14300</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A117" t="s">
+        <v>398</v>
+      </c>
+      <c r="B117">
+        <v>14500</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A118" t="s">
+        <v>401</v>
+      </c>
+      <c r="B118">
+        <v>14600</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A119" t="s">
+        <v>398</v>
+      </c>
+      <c r="B119">
+        <v>14700</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B120">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A121" t="s">
+        <v>398</v>
+      </c>
+      <c r="B121">
+        <v>15100</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A122" t="s">
+        <v>398</v>
+      </c>
+      <c r="B122">
+        <v>15700</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A123" t="s">
+        <v>398</v>
+      </c>
+      <c r="B123">
+        <v>15800</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B124">
+        <v>16800</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B125">
+        <v>16900</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B126">
+        <v>17700</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B127">
+        <v>17800</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B128">
+        <v>18100</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B129">
+        <v>18800</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B130">
+        <v>19000</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B131">
+        <v>19300</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B132">
+        <v>19900</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A133" t="s">
+        <v>392</v>
+      </c>
+      <c r="B133">
+        <v>21100</v>
+      </c>
+      <c r="C133" s="20">
+        <v>21168</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A134" t="s">
+        <v>411</v>
+      </c>
+      <c r="B134" t="s">
+        <v>412</v>
+      </c>
+      <c r="C134" s="20" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A135" t="s">
+        <v>16</v>
+      </c>
+      <c r="B135" t="s">
+        <v>412</v>
+      </c>
+      <c r="C135" s="20" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A136" t="s">
+        <v>153</v>
+      </c>
+      <c r="B136" t="s">
+        <v>21</v>
+      </c>
+      <c r="C136" s="20" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A137" t="s">
+        <v>413</v>
+      </c>
+      <c r="B137" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A138" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A139" t="s">
+        <v>45</v>
+      </c>
+      <c r="B139" t="s">
+        <v>412</v>
+      </c>
+      <c r="C139" s="20" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A140" t="s">
+        <v>18</v>
+      </c>
+      <c r="B140" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A141" t="s">
+        <v>16</v>
+      </c>
+      <c r="B141" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A142" t="s">
+        <v>17</v>
+      </c>
+      <c r="B142" t="s">
+        <v>424</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:D138" xr:uid="{A1F2546F-C082-477C-B976-7FC2D49CF31C}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D138">
+      <sortCondition ref="B1:B138"/>
+    </sortState>
+  </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D116"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C117" sqref="C117"/>
+    <sheetView topLeftCell="A85" workbookViewId="0">
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -7550,11 +8803,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0211A2A-DC69-448E-B36B-BE6820863E81}">
   <dimension ref="A1:C100"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C27" sqref="A27:C28"/>
     </sheetView>
   </sheetViews>
@@ -8616,11 +9869,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{778DD009-53DD-426B-BBA7-ABCE73A49F39}">
   <dimension ref="A1:C108"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -9520,11 +10773,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{379E3CDC-714A-4865-8067-4D8FDE224D87}">
   <dimension ref="A1:I52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
@@ -10384,11 +11637,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DB840A4-93DF-43F4-B9FF-1DFD0858F8C3}">
   <dimension ref="A1:H562"/>
   <sheetViews>
-    <sheetView topLeftCell="A154" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I163" sqref="I163"/>
     </sheetView>
   </sheetViews>
@@ -20168,4 +21421,1479 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId370"/>
   <legacyDrawing r:id="rId371"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5776901-1A98-4DFB-9BF8-9460FA86F060}">
+  <dimension ref="A1:BG22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="X25" sqref="X25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="2" width="2.59765625" customWidth="1"/>
+    <col min="3" max="3" width="12.06640625" customWidth="1"/>
+    <col min="4" max="59" width="2.59765625" style="13" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:59" ht="26.25" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="13">
+        <v>1970</v>
+      </c>
+      <c r="E1" s="13">
+        <v>1971</v>
+      </c>
+      <c r="F1" s="13">
+        <v>1972</v>
+      </c>
+      <c r="G1" s="13">
+        <v>1973</v>
+      </c>
+      <c r="H1" s="13">
+        <v>1974</v>
+      </c>
+      <c r="I1" s="13">
+        <v>1975</v>
+      </c>
+      <c r="J1" s="13">
+        <v>1976</v>
+      </c>
+      <c r="K1" s="13">
+        <v>1977</v>
+      </c>
+      <c r="L1" s="13">
+        <v>1978</v>
+      </c>
+      <c r="M1" s="13">
+        <v>1979</v>
+      </c>
+      <c r="N1" s="13">
+        <v>1980</v>
+      </c>
+      <c r="O1" s="13">
+        <v>1981</v>
+      </c>
+      <c r="P1" s="13">
+        <v>1982</v>
+      </c>
+      <c r="Q1" s="13">
+        <v>1983</v>
+      </c>
+      <c r="R1" s="13">
+        <v>1984</v>
+      </c>
+      <c r="S1" s="13">
+        <v>1985</v>
+      </c>
+      <c r="T1" s="13">
+        <v>1986</v>
+      </c>
+      <c r="U1" s="13">
+        <v>1987</v>
+      </c>
+      <c r="V1" s="13">
+        <v>1988</v>
+      </c>
+      <c r="W1" s="13">
+        <v>1989</v>
+      </c>
+      <c r="X1" s="13">
+        <v>1990</v>
+      </c>
+      <c r="Y1" s="13">
+        <v>1991</v>
+      </c>
+      <c r="Z1" s="13">
+        <v>1992</v>
+      </c>
+      <c r="AA1" s="13">
+        <v>1993</v>
+      </c>
+      <c r="AB1" s="13">
+        <v>1994</v>
+      </c>
+      <c r="AC1" s="13">
+        <v>1995</v>
+      </c>
+      <c r="AD1" s="13">
+        <v>1996</v>
+      </c>
+      <c r="AE1" s="13">
+        <v>1997</v>
+      </c>
+      <c r="AF1" s="13">
+        <v>1998</v>
+      </c>
+      <c r="AG1" s="13">
+        <v>1999</v>
+      </c>
+      <c r="AH1" s="13">
+        <v>2000</v>
+      </c>
+      <c r="AI1" s="13">
+        <v>2001</v>
+      </c>
+      <c r="AJ1" s="13">
+        <v>2002</v>
+      </c>
+      <c r="AK1" s="13">
+        <v>2003</v>
+      </c>
+      <c r="AL1" s="13">
+        <v>2004</v>
+      </c>
+      <c r="AM1" s="13">
+        <v>2005</v>
+      </c>
+      <c r="AN1" s="13">
+        <v>2006</v>
+      </c>
+      <c r="AO1" s="13">
+        <v>2007</v>
+      </c>
+      <c r="AP1" s="13">
+        <v>2008</v>
+      </c>
+      <c r="AQ1" s="13">
+        <v>2009</v>
+      </c>
+      <c r="AR1" s="13">
+        <v>2010</v>
+      </c>
+      <c r="AS1" s="13">
+        <v>2011</v>
+      </c>
+      <c r="AT1" s="13">
+        <v>2012</v>
+      </c>
+      <c r="AU1" s="13">
+        <v>2013</v>
+      </c>
+      <c r="AV1" s="13">
+        <v>2014</v>
+      </c>
+      <c r="AW1" s="13">
+        <v>2015</v>
+      </c>
+      <c r="AX1" s="13">
+        <v>2016</v>
+      </c>
+      <c r="AY1" s="13">
+        <v>2017</v>
+      </c>
+      <c r="AZ1" s="13">
+        <v>2018</v>
+      </c>
+      <c r="BA1" s="13">
+        <v>2019</v>
+      </c>
+      <c r="BB1" s="13">
+        <v>2020</v>
+      </c>
+      <c r="BC1" s="13">
+        <v>2021</v>
+      </c>
+      <c r="BD1" s="13">
+        <v>2022</v>
+      </c>
+      <c r="BE1" s="13">
+        <v>2023</v>
+      </c>
+      <c r="BF1" s="13">
+        <v>2024</v>
+      </c>
+      <c r="BG1" s="13">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="2" spans="1:59" x14ac:dyDescent="0.45">
+      <c r="A2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="17"/>
+      <c r="L2" s="17"/>
+      <c r="M2" s="17"/>
+      <c r="N2" s="17"/>
+      <c r="O2" s="17"/>
+      <c r="P2" s="17"/>
+      <c r="Q2" s="17"/>
+      <c r="R2" s="17"/>
+      <c r="S2" s="17"/>
+      <c r="T2" s="17"/>
+      <c r="U2" s="17"/>
+      <c r="V2" s="17"/>
+      <c r="W2" s="17"/>
+      <c r="X2" s="17"/>
+      <c r="Y2" s="17"/>
+      <c r="Z2" s="17"/>
+      <c r="AA2" s="17"/>
+      <c r="AB2" s="17"/>
+      <c r="AC2" s="17"/>
+      <c r="AD2" s="17"/>
+      <c r="AE2" s="17"/>
+      <c r="AF2" s="17"/>
+      <c r="AG2" s="17"/>
+      <c r="AH2" s="17"/>
+      <c r="AI2" s="17"/>
+      <c r="AJ2" s="17"/>
+      <c r="AK2" s="17"/>
+      <c r="AL2" s="17"/>
+      <c r="AM2" s="17"/>
+      <c r="AN2" s="17"/>
+      <c r="AO2" s="17"/>
+      <c r="AP2" s="17"/>
+      <c r="AQ2" s="17"/>
+      <c r="AR2" s="17"/>
+      <c r="AS2" s="17"/>
+      <c r="AT2" s="17"/>
+      <c r="AU2" s="17"/>
+      <c r="AV2" s="17"/>
+      <c r="AW2" s="17"/>
+      <c r="AX2" s="17"/>
+      <c r="AY2" s="17"/>
+      <c r="AZ2" s="17"/>
+      <c r="BA2" s="17"/>
+      <c r="BB2" s="17"/>
+      <c r="BC2" s="17"/>
+      <c r="BD2" s="17"/>
+      <c r="BE2" s="17"/>
+      <c r="BF2" s="17"/>
+      <c r="BG2" s="17"/>
+    </row>
+    <row r="3" spans="1:59" x14ac:dyDescent="0.45">
+      <c r="B3" t="s">
+        <v>283</v>
+      </c>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="17"/>
+      <c r="K3" s="17"/>
+      <c r="L3" s="17"/>
+      <c r="M3" s="17"/>
+      <c r="N3" s="17"/>
+      <c r="O3" s="17"/>
+      <c r="P3" s="17"/>
+      <c r="Q3" s="17"/>
+      <c r="R3" s="17"/>
+      <c r="S3" s="17"/>
+      <c r="T3" s="17"/>
+      <c r="U3" s="17"/>
+      <c r="V3" s="17"/>
+      <c r="W3" s="17"/>
+      <c r="X3" s="17"/>
+      <c r="Y3" s="17"/>
+      <c r="Z3" s="17"/>
+      <c r="AA3" s="17"/>
+      <c r="AB3" s="17"/>
+      <c r="AC3" s="17"/>
+      <c r="AD3" s="17"/>
+      <c r="AE3" s="17"/>
+      <c r="AF3" s="17"/>
+      <c r="AG3" s="17"/>
+      <c r="AH3" s="17"/>
+      <c r="AI3" s="17"/>
+      <c r="AJ3" s="17"/>
+      <c r="AK3" s="17"/>
+      <c r="AL3" s="17"/>
+      <c r="AM3" s="17"/>
+      <c r="AN3" s="17"/>
+      <c r="AO3" s="17"/>
+      <c r="AP3" s="17"/>
+      <c r="AQ3" s="17"/>
+      <c r="AR3" s="17"/>
+      <c r="AS3" s="17"/>
+      <c r="AT3" s="17"/>
+      <c r="AU3" s="17"/>
+      <c r="AV3" s="17"/>
+      <c r="AW3" s="17"/>
+      <c r="AX3" s="17"/>
+      <c r="AY3" s="17"/>
+      <c r="AZ3" s="17"/>
+      <c r="BA3" s="17"/>
+      <c r="BB3" s="17"/>
+      <c r="BC3" s="17"/>
+      <c r="BD3" s="17"/>
+      <c r="BE3" s="17"/>
+      <c r="BF3" s="17"/>
+      <c r="BG3" s="17"/>
+    </row>
+    <row r="4" spans="1:59" x14ac:dyDescent="0.45">
+      <c r="C4" t="s">
+        <v>384</v>
+      </c>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="15"/>
+      <c r="K4" s="15"/>
+      <c r="L4" s="15"/>
+      <c r="M4" s="15"/>
+      <c r="N4" s="15"/>
+      <c r="O4" s="15"/>
+      <c r="P4" s="15"/>
+      <c r="Q4" s="15"/>
+      <c r="R4" s="15"/>
+      <c r="S4" s="15"/>
+      <c r="T4" s="15"/>
+      <c r="U4" s="15"/>
+      <c r="V4" s="15"/>
+      <c r="W4" s="15"/>
+      <c r="X4" s="15"/>
+      <c r="Y4" s="15"/>
+      <c r="Z4" s="15"/>
+      <c r="AA4" s="15"/>
+      <c r="AB4" s="15"/>
+      <c r="AC4" s="15"/>
+      <c r="AD4" s="15"/>
+      <c r="AE4" s="15"/>
+      <c r="AF4" s="15"/>
+      <c r="AG4" s="15"/>
+      <c r="AH4" s="15"/>
+      <c r="AI4" s="15"/>
+      <c r="AJ4" s="15"/>
+      <c r="AK4" s="15"/>
+      <c r="AL4" s="15"/>
+      <c r="AM4" s="15"/>
+      <c r="AN4" s="15"/>
+      <c r="AO4" s="15"/>
+      <c r="AP4" s="15"/>
+      <c r="AQ4" s="15"/>
+      <c r="AR4" s="15"/>
+      <c r="AS4" s="15"/>
+      <c r="AT4" s="15"/>
+      <c r="AU4" s="15"/>
+      <c r="AV4" s="15"/>
+      <c r="AW4" s="15"/>
+      <c r="AX4" s="15"/>
+      <c r="AY4" s="15"/>
+      <c r="AZ4" s="15"/>
+      <c r="BA4" s="15"/>
+      <c r="BB4" s="15"/>
+      <c r="BC4" s="15"/>
+      <c r="BD4" s="15"/>
+      <c r="BE4" s="15"/>
+      <c r="BF4" s="15"/>
+      <c r="BG4" s="15"/>
+    </row>
+    <row r="5" spans="1:59" x14ac:dyDescent="0.45">
+      <c r="C5" t="s">
+        <v>385</v>
+      </c>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="14"/>
+      <c r="M5" s="14"/>
+      <c r="N5" s="14"/>
+      <c r="O5" s="14"/>
+      <c r="P5" s="14"/>
+      <c r="Q5" s="14"/>
+      <c r="R5" s="14"/>
+      <c r="S5" s="14"/>
+      <c r="T5" s="14"/>
+      <c r="U5" s="14"/>
+      <c r="V5" s="14"/>
+      <c r="W5" s="14"/>
+      <c r="X5" s="14"/>
+      <c r="Y5" s="14"/>
+      <c r="Z5" s="14"/>
+      <c r="AA5" s="14"/>
+      <c r="AB5" s="14"/>
+      <c r="AC5" s="14"/>
+      <c r="AD5" s="14"/>
+      <c r="AE5" s="14"/>
+      <c r="AF5" s="14"/>
+      <c r="AG5" s="14"/>
+      <c r="AH5" s="14"/>
+      <c r="AI5" s="14"/>
+      <c r="AJ5" s="14"/>
+      <c r="AK5" s="14"/>
+      <c r="AL5" s="14"/>
+      <c r="AM5" s="14"/>
+      <c r="AN5" s="14"/>
+      <c r="AO5" s="14"/>
+      <c r="AP5" s="14"/>
+      <c r="AQ5" s="14"/>
+      <c r="AR5" s="14"/>
+      <c r="AS5" s="14"/>
+      <c r="AT5" s="14"/>
+      <c r="AU5" s="14"/>
+      <c r="AV5" s="14"/>
+      <c r="AW5" s="14"/>
+      <c r="AX5" s="14"/>
+      <c r="AY5" s="15"/>
+      <c r="AZ5" s="15"/>
+      <c r="BA5" s="15"/>
+      <c r="BB5" s="15"/>
+      <c r="BC5" s="15"/>
+      <c r="BD5" s="15"/>
+      <c r="BE5" s="15"/>
+      <c r="BF5" s="15"/>
+      <c r="BG5" s="15"/>
+    </row>
+    <row r="6" spans="1:59" x14ac:dyDescent="0.45">
+      <c r="C6" t="s">
+        <v>382</v>
+      </c>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="15"/>
+      <c r="M6" s="15"/>
+      <c r="N6" s="15"/>
+      <c r="O6" s="15"/>
+      <c r="P6" s="15"/>
+      <c r="Q6" s="15"/>
+      <c r="R6" s="15"/>
+      <c r="S6" s="15"/>
+      <c r="T6" s="15"/>
+      <c r="U6" s="15"/>
+      <c r="V6" s="15"/>
+      <c r="W6" s="15"/>
+      <c r="X6" s="15"/>
+      <c r="Y6" s="15"/>
+      <c r="Z6" s="15"/>
+      <c r="AA6" s="15"/>
+      <c r="AB6" s="15"/>
+      <c r="AC6" s="14"/>
+      <c r="AD6" s="14"/>
+      <c r="AE6" s="15"/>
+      <c r="AF6" s="15"/>
+      <c r="AG6" s="15"/>
+      <c r="AH6" s="15"/>
+      <c r="AI6" s="15"/>
+      <c r="AJ6" s="15"/>
+      <c r="AK6" s="15"/>
+      <c r="AL6" s="15"/>
+      <c r="AM6" s="15"/>
+      <c r="AN6" s="15"/>
+      <c r="AO6" s="15"/>
+      <c r="AP6" s="15"/>
+      <c r="AQ6" s="15"/>
+      <c r="AR6" s="15"/>
+      <c r="AS6" s="15"/>
+      <c r="AT6" s="15"/>
+      <c r="AU6" s="15"/>
+      <c r="AV6" s="15"/>
+      <c r="AW6" s="15"/>
+      <c r="AX6" s="15"/>
+      <c r="AY6" s="15"/>
+      <c r="AZ6" s="15"/>
+      <c r="BA6" s="15"/>
+      <c r="BB6" s="15"/>
+      <c r="BC6" s="15"/>
+      <c r="BD6" s="15"/>
+      <c r="BE6" s="15"/>
+      <c r="BF6" s="15"/>
+      <c r="BG6" s="15"/>
+    </row>
+    <row r="7" spans="1:59" x14ac:dyDescent="0.45">
+      <c r="C7" t="s">
+        <v>383</v>
+      </c>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="15"/>
+      <c r="K7" s="15"/>
+      <c r="L7" s="15"/>
+      <c r="M7" s="15"/>
+      <c r="N7" s="15"/>
+      <c r="O7" s="15"/>
+      <c r="P7" s="15"/>
+      <c r="Q7" s="15"/>
+      <c r="R7" s="15"/>
+      <c r="S7" s="15"/>
+      <c r="T7" s="15"/>
+      <c r="U7" s="15"/>
+      <c r="V7" s="15"/>
+      <c r="W7" s="15"/>
+      <c r="X7" s="15"/>
+      <c r="Y7" s="15"/>
+      <c r="Z7" s="15"/>
+      <c r="AA7" s="15"/>
+      <c r="AB7" s="15"/>
+      <c r="AC7" s="15"/>
+      <c r="AD7" s="15"/>
+      <c r="AE7" s="15"/>
+      <c r="AF7" s="15"/>
+      <c r="AG7" s="15"/>
+      <c r="AH7" s="15"/>
+      <c r="AI7" s="15"/>
+      <c r="AJ7" s="15"/>
+      <c r="AK7" s="15"/>
+      <c r="AL7" s="14"/>
+      <c r="AM7" s="16"/>
+      <c r="AN7" s="16"/>
+      <c r="AO7" s="16"/>
+      <c r="AP7" s="16"/>
+      <c r="AQ7" s="16"/>
+      <c r="AR7" s="15"/>
+      <c r="AS7" s="15"/>
+      <c r="AT7" s="15"/>
+      <c r="AU7" s="15"/>
+      <c r="AV7" s="15"/>
+      <c r="AW7" s="15"/>
+      <c r="AX7" s="15"/>
+      <c r="AY7" s="15"/>
+      <c r="AZ7" s="15"/>
+      <c r="BA7" s="15"/>
+      <c r="BB7" s="15"/>
+      <c r="BC7" s="15"/>
+      <c r="BD7" s="15"/>
+      <c r="BE7" s="15"/>
+      <c r="BF7" s="15"/>
+      <c r="BG7" s="15"/>
+    </row>
+    <row r="8" spans="1:59" x14ac:dyDescent="0.45">
+      <c r="B8" t="s">
+        <v>379</v>
+      </c>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="15"/>
+      <c r="L8" s="15"/>
+      <c r="M8" s="15"/>
+      <c r="N8" s="15"/>
+      <c r="O8" s="15"/>
+      <c r="P8" s="15"/>
+      <c r="Q8" s="15"/>
+      <c r="R8" s="15"/>
+      <c r="S8" s="15"/>
+      <c r="T8" s="15"/>
+      <c r="U8" s="15"/>
+      <c r="V8" s="15"/>
+      <c r="W8" s="15"/>
+      <c r="X8" s="15"/>
+      <c r="Y8" s="15"/>
+      <c r="Z8" s="15"/>
+      <c r="AA8" s="15"/>
+      <c r="AB8" s="15"/>
+      <c r="AC8" s="15"/>
+      <c r="AD8" s="15"/>
+      <c r="AE8" s="15"/>
+      <c r="AF8" s="15"/>
+      <c r="AG8" s="15"/>
+      <c r="AH8" s="15"/>
+      <c r="AI8" s="15"/>
+      <c r="AJ8" s="15"/>
+      <c r="AK8" s="15"/>
+      <c r="AL8" s="15"/>
+      <c r="AM8" s="15"/>
+      <c r="AN8" s="14"/>
+      <c r="AO8" s="14"/>
+      <c r="AP8" s="14"/>
+      <c r="AQ8" s="15"/>
+      <c r="AR8" s="15"/>
+      <c r="AS8" s="15"/>
+      <c r="AT8" s="15"/>
+      <c r="AU8" s="15"/>
+      <c r="AV8" s="15"/>
+      <c r="AW8" s="15"/>
+      <c r="AX8" s="15"/>
+      <c r="AY8" s="15"/>
+      <c r="AZ8" s="15"/>
+      <c r="BA8" s="15"/>
+      <c r="BB8" s="15"/>
+      <c r="BC8" s="15"/>
+      <c r="BD8" s="15"/>
+      <c r="BE8" s="15"/>
+      <c r="BF8" s="15"/>
+      <c r="BG8" s="15"/>
+    </row>
+    <row r="9" spans="1:59" x14ac:dyDescent="0.45">
+      <c r="B9" t="s">
+        <v>380</v>
+      </c>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="15"/>
+      <c r="M9" s="15"/>
+      <c r="N9" s="15"/>
+      <c r="O9" s="15"/>
+      <c r="P9" s="15"/>
+      <c r="Q9" s="15"/>
+      <c r="R9" s="15"/>
+      <c r="S9" s="15"/>
+      <c r="T9" s="15"/>
+      <c r="U9" s="15"/>
+      <c r="V9" s="15"/>
+      <c r="W9" s="15"/>
+      <c r="X9" s="15"/>
+      <c r="Y9" s="15"/>
+      <c r="Z9" s="15"/>
+      <c r="AA9" s="15"/>
+      <c r="AB9" s="15"/>
+      <c r="AC9" s="15"/>
+      <c r="AD9" s="15"/>
+      <c r="AE9" s="15"/>
+      <c r="AF9" s="15"/>
+      <c r="AG9" s="15"/>
+      <c r="AH9" s="15"/>
+      <c r="AI9" s="15"/>
+      <c r="AJ9" s="15"/>
+      <c r="AK9" s="15"/>
+      <c r="AL9" s="15"/>
+      <c r="AM9" s="15"/>
+      <c r="AN9" s="14"/>
+      <c r="AO9" s="14"/>
+      <c r="AP9" s="14"/>
+      <c r="AQ9" s="14"/>
+      <c r="AR9" s="14"/>
+      <c r="AS9" s="14"/>
+      <c r="AT9" s="14"/>
+      <c r="AU9" s="14"/>
+      <c r="AV9" s="15"/>
+      <c r="AW9" s="15"/>
+      <c r="AX9" s="15"/>
+      <c r="AY9" s="15"/>
+      <c r="AZ9" s="15"/>
+      <c r="BA9" s="15"/>
+      <c r="BB9" s="15"/>
+      <c r="BC9" s="15"/>
+      <c r="BD9" s="15"/>
+      <c r="BE9" s="15"/>
+      <c r="BF9" s="15"/>
+      <c r="BG9" s="15"/>
+    </row>
+    <row r="10" spans="1:59" x14ac:dyDescent="0.45">
+      <c r="B10" t="s">
+        <v>381</v>
+      </c>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="15"/>
+      <c r="K10" s="15"/>
+      <c r="L10" s="15"/>
+      <c r="M10" s="15"/>
+      <c r="N10" s="15"/>
+      <c r="O10" s="15"/>
+      <c r="P10" s="15"/>
+      <c r="Q10" s="15"/>
+      <c r="R10" s="15"/>
+      <c r="S10" s="15"/>
+      <c r="T10" s="15"/>
+      <c r="U10" s="15"/>
+      <c r="V10" s="15"/>
+      <c r="W10" s="15"/>
+      <c r="X10" s="15"/>
+      <c r="Y10" s="15"/>
+      <c r="Z10" s="15"/>
+      <c r="AA10" s="15"/>
+      <c r="AB10" s="15"/>
+      <c r="AC10" s="15"/>
+      <c r="AD10" s="15"/>
+      <c r="AE10" s="15"/>
+      <c r="AF10" s="15"/>
+      <c r="AG10" s="15"/>
+      <c r="AH10" s="15"/>
+      <c r="AI10" s="15"/>
+      <c r="AJ10" s="15"/>
+      <c r="AK10" s="15"/>
+      <c r="AL10" s="15"/>
+      <c r="AM10" s="15"/>
+      <c r="AN10" s="14"/>
+      <c r="AO10" s="14"/>
+      <c r="AP10" s="14"/>
+      <c r="AQ10" s="15"/>
+      <c r="AR10" s="15"/>
+      <c r="AS10" s="15"/>
+      <c r="AT10" s="15"/>
+      <c r="AU10" s="15"/>
+      <c r="AV10" s="15"/>
+      <c r="AW10" s="15"/>
+      <c r="AX10" s="15"/>
+      <c r="AY10" s="15"/>
+      <c r="AZ10" s="15"/>
+      <c r="BA10" s="15"/>
+      <c r="BB10" s="15"/>
+      <c r="BC10" s="15"/>
+      <c r="BD10" s="15"/>
+      <c r="BE10" s="15"/>
+      <c r="BF10" s="15"/>
+      <c r="BG10" s="15"/>
+    </row>
+    <row r="11" spans="1:59" x14ac:dyDescent="0.45">
+      <c r="A11" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="17"/>
+      <c r="I11" s="17"/>
+      <c r="J11" s="17"/>
+      <c r="K11" s="17"/>
+      <c r="L11" s="17"/>
+      <c r="M11" s="17"/>
+      <c r="N11" s="17"/>
+      <c r="O11" s="17"/>
+      <c r="P11" s="17"/>
+      <c r="Q11" s="17"/>
+      <c r="R11" s="17"/>
+      <c r="S11" s="17"/>
+      <c r="T11" s="17"/>
+      <c r="U11" s="17"/>
+      <c r="V11" s="17"/>
+      <c r="W11" s="17"/>
+      <c r="X11" s="17"/>
+      <c r="Y11" s="17"/>
+      <c r="Z11" s="17"/>
+      <c r="AA11" s="17"/>
+      <c r="AB11" s="17"/>
+      <c r="AC11" s="17"/>
+      <c r="AD11" s="17"/>
+      <c r="AE11" s="17"/>
+      <c r="AF11" s="17"/>
+      <c r="AG11" s="17"/>
+      <c r="AH11" s="17"/>
+      <c r="AI11" s="17"/>
+      <c r="AJ11" s="17"/>
+      <c r="AK11" s="17"/>
+      <c r="AL11" s="17"/>
+      <c r="AM11" s="17"/>
+      <c r="AN11" s="17"/>
+      <c r="AO11" s="17"/>
+      <c r="AP11" s="17"/>
+      <c r="AQ11" s="17"/>
+      <c r="AR11" s="17"/>
+      <c r="AS11" s="17"/>
+      <c r="AT11" s="17"/>
+      <c r="AU11" s="17"/>
+      <c r="AV11" s="17"/>
+      <c r="AW11" s="17"/>
+      <c r="AX11" s="17"/>
+      <c r="AY11" s="17"/>
+      <c r="AZ11" s="17"/>
+      <c r="BA11" s="17"/>
+      <c r="BB11" s="17"/>
+      <c r="BC11" s="17"/>
+      <c r="BD11" s="17"/>
+      <c r="BE11" s="17"/>
+      <c r="BF11" s="17"/>
+      <c r="BG11" s="17"/>
+    </row>
+    <row r="12" spans="1:59" x14ac:dyDescent="0.45">
+      <c r="B12" t="s">
+        <v>283</v>
+      </c>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="17"/>
+      <c r="I12" s="17"/>
+      <c r="J12" s="17"/>
+      <c r="K12" s="17"/>
+      <c r="L12" s="17"/>
+      <c r="M12" s="17"/>
+      <c r="N12" s="17"/>
+      <c r="O12" s="17"/>
+      <c r="P12" s="17"/>
+      <c r="Q12" s="17"/>
+      <c r="R12" s="17"/>
+      <c r="S12" s="17"/>
+      <c r="T12" s="17"/>
+      <c r="U12" s="17"/>
+      <c r="V12" s="17"/>
+      <c r="W12" s="17"/>
+      <c r="X12" s="17"/>
+      <c r="Y12" s="17"/>
+      <c r="Z12" s="17"/>
+      <c r="AA12" s="17"/>
+      <c r="AB12" s="17"/>
+      <c r="AC12" s="17"/>
+      <c r="AD12" s="17"/>
+      <c r="AE12" s="17"/>
+      <c r="AF12" s="17"/>
+      <c r="AG12" s="17"/>
+      <c r="AH12" s="17"/>
+      <c r="AI12" s="17"/>
+      <c r="AJ12" s="17"/>
+      <c r="AK12" s="17"/>
+      <c r="AL12" s="17"/>
+      <c r="AM12" s="17"/>
+      <c r="AN12" s="17"/>
+      <c r="AO12" s="17"/>
+      <c r="AP12" s="17"/>
+      <c r="AQ12" s="17"/>
+      <c r="AR12" s="17"/>
+      <c r="AS12" s="17"/>
+      <c r="AT12" s="17"/>
+      <c r="AU12" s="17"/>
+      <c r="AV12" s="17"/>
+      <c r="AW12" s="17"/>
+      <c r="AX12" s="17"/>
+      <c r="AY12" s="17"/>
+      <c r="AZ12" s="17"/>
+      <c r="BA12" s="17"/>
+      <c r="BB12" s="17"/>
+      <c r="BC12" s="17"/>
+      <c r="BD12" s="17"/>
+      <c r="BE12" s="17"/>
+      <c r="BF12" s="17"/>
+      <c r="BG12" s="17"/>
+    </row>
+    <row r="13" spans="1:59" x14ac:dyDescent="0.45">
+      <c r="C13" t="s">
+        <v>384</v>
+      </c>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="15"/>
+      <c r="K13" s="15"/>
+      <c r="L13" s="15"/>
+      <c r="M13" s="15"/>
+      <c r="N13" s="15"/>
+      <c r="O13" s="15"/>
+      <c r="P13" s="15"/>
+      <c r="Q13" s="15"/>
+      <c r="R13" s="15"/>
+      <c r="S13" s="15"/>
+      <c r="T13" s="15"/>
+      <c r="U13" s="15"/>
+      <c r="V13" s="15"/>
+      <c r="W13" s="15"/>
+      <c r="X13" s="15"/>
+      <c r="Y13" s="15"/>
+      <c r="Z13" s="15"/>
+      <c r="AA13" s="15"/>
+      <c r="AB13" s="15"/>
+      <c r="AC13" s="15"/>
+      <c r="AD13" s="15"/>
+      <c r="AE13" s="15"/>
+      <c r="AF13" s="15"/>
+      <c r="AG13" s="15"/>
+      <c r="AH13" s="15"/>
+      <c r="AI13" s="15"/>
+      <c r="AJ13" s="15"/>
+      <c r="AK13" s="15"/>
+      <c r="AL13" s="15"/>
+      <c r="AM13" s="15"/>
+      <c r="AN13" s="15"/>
+      <c r="AO13" s="15"/>
+      <c r="AP13" s="15"/>
+      <c r="AQ13" s="15"/>
+      <c r="AR13" s="15"/>
+      <c r="AS13" s="15"/>
+      <c r="AT13" s="15"/>
+      <c r="AU13" s="15"/>
+      <c r="AV13" s="15"/>
+      <c r="AW13" s="15"/>
+      <c r="AX13" s="15"/>
+      <c r="AY13" s="15"/>
+      <c r="AZ13" s="15"/>
+      <c r="BA13" s="15"/>
+      <c r="BB13" s="15"/>
+      <c r="BC13" s="15"/>
+      <c r="BD13" s="15"/>
+      <c r="BE13" s="15"/>
+      <c r="BF13" s="15"/>
+      <c r="BG13" s="15"/>
+    </row>
+    <row r="14" spans="1:59" x14ac:dyDescent="0.45">
+      <c r="C14" t="s">
+        <v>385</v>
+      </c>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="14"/>
+      <c r="L14" s="14"/>
+      <c r="M14" s="14"/>
+      <c r="N14" s="14"/>
+      <c r="O14" s="14"/>
+      <c r="P14" s="14"/>
+      <c r="Q14" s="14"/>
+      <c r="R14" s="14"/>
+      <c r="S14" s="14"/>
+      <c r="T14" s="14"/>
+      <c r="U14" s="14"/>
+      <c r="V14" s="14"/>
+      <c r="W14" s="14"/>
+      <c r="X14" s="14"/>
+      <c r="Y14" s="14"/>
+      <c r="Z14" s="14"/>
+      <c r="AA14" s="14"/>
+      <c r="AB14" s="14"/>
+      <c r="AC14" s="14"/>
+      <c r="AD14" s="14"/>
+      <c r="AE14" s="14"/>
+      <c r="AF14" s="14"/>
+      <c r="AG14" s="14"/>
+      <c r="AH14" s="14"/>
+      <c r="AI14" s="14"/>
+      <c r="AJ14" s="14"/>
+      <c r="AK14" s="14"/>
+      <c r="AL14" s="14"/>
+      <c r="AM14" s="14"/>
+      <c r="AN14" s="14"/>
+      <c r="AO14" s="14"/>
+      <c r="AP14" s="14"/>
+      <c r="AQ14" s="14"/>
+      <c r="AR14" s="14"/>
+      <c r="AS14" s="15"/>
+      <c r="AT14" s="15"/>
+      <c r="AU14" s="15"/>
+      <c r="AV14" s="15"/>
+      <c r="AW14" s="15"/>
+      <c r="AX14" s="15"/>
+      <c r="AY14" s="15"/>
+      <c r="AZ14" s="15"/>
+      <c r="BA14" s="15"/>
+      <c r="BB14" s="15"/>
+      <c r="BC14" s="15"/>
+      <c r="BD14" s="15"/>
+      <c r="BE14" s="15"/>
+      <c r="BF14" s="15"/>
+      <c r="BG14" s="15"/>
+    </row>
+    <row r="15" spans="1:59" x14ac:dyDescent="0.45">
+      <c r="A15" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="17"/>
+      <c r="J15" s="17"/>
+      <c r="K15" s="17"/>
+      <c r="L15" s="17"/>
+      <c r="M15" s="17"/>
+      <c r="N15" s="17"/>
+      <c r="O15" s="17"/>
+      <c r="P15" s="17"/>
+      <c r="Q15" s="17"/>
+      <c r="R15" s="17"/>
+      <c r="S15" s="17"/>
+      <c r="T15" s="17"/>
+      <c r="U15" s="17"/>
+      <c r="V15" s="17"/>
+      <c r="W15" s="17"/>
+      <c r="X15" s="17"/>
+      <c r="Y15" s="17"/>
+      <c r="Z15" s="17"/>
+      <c r="AA15" s="17"/>
+      <c r="AB15" s="17"/>
+      <c r="AC15" s="17"/>
+      <c r="AD15" s="17"/>
+      <c r="AE15" s="17"/>
+      <c r="AF15" s="17"/>
+      <c r="AG15" s="17"/>
+      <c r="AH15" s="17"/>
+      <c r="AI15" s="17"/>
+      <c r="AJ15" s="17"/>
+      <c r="AK15" s="17"/>
+      <c r="AL15" s="17"/>
+      <c r="AM15" s="17"/>
+      <c r="AN15" s="17"/>
+      <c r="AO15" s="17"/>
+      <c r="AP15" s="17"/>
+      <c r="AQ15" s="17"/>
+      <c r="AR15" s="17"/>
+      <c r="AS15" s="17"/>
+      <c r="AT15" s="17"/>
+      <c r="AU15" s="17"/>
+      <c r="AV15" s="17"/>
+      <c r="AW15" s="17"/>
+      <c r="AX15" s="17"/>
+      <c r="AY15" s="17"/>
+      <c r="AZ15" s="17"/>
+      <c r="BA15" s="17"/>
+      <c r="BB15" s="17"/>
+      <c r="BC15" s="17"/>
+      <c r="BD15" s="17"/>
+      <c r="BE15" s="17"/>
+      <c r="BF15" s="17"/>
+      <c r="BG15" s="17"/>
+    </row>
+    <row r="16" spans="1:59" x14ac:dyDescent="0.45">
+      <c r="B16" t="s">
+        <v>283</v>
+      </c>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="17"/>
+      <c r="I16" s="17"/>
+      <c r="J16" s="17"/>
+      <c r="K16" s="17"/>
+      <c r="L16" s="17"/>
+      <c r="M16" s="17"/>
+      <c r="N16" s="17"/>
+      <c r="O16" s="17"/>
+      <c r="P16" s="17"/>
+      <c r="Q16" s="17"/>
+      <c r="R16" s="17"/>
+      <c r="S16" s="17"/>
+      <c r="T16" s="17"/>
+      <c r="U16" s="17"/>
+      <c r="V16" s="17"/>
+      <c r="W16" s="17"/>
+      <c r="X16" s="17"/>
+      <c r="Y16" s="17"/>
+      <c r="Z16" s="17"/>
+      <c r="AA16" s="17"/>
+      <c r="AB16" s="17"/>
+      <c r="AC16" s="17"/>
+      <c r="AD16" s="17"/>
+      <c r="AE16" s="17"/>
+      <c r="AF16" s="17"/>
+      <c r="AG16" s="17"/>
+      <c r="AH16" s="17"/>
+      <c r="AI16" s="17"/>
+      <c r="AJ16" s="17"/>
+      <c r="AK16" s="17"/>
+      <c r="AL16" s="17"/>
+      <c r="AM16" s="17"/>
+      <c r="AN16" s="17"/>
+      <c r="AO16" s="17"/>
+      <c r="AP16" s="17"/>
+      <c r="AQ16" s="17"/>
+      <c r="AR16" s="17"/>
+      <c r="AS16" s="17"/>
+      <c r="AT16" s="17"/>
+      <c r="AU16" s="17"/>
+      <c r="AV16" s="17"/>
+      <c r="AW16" s="17"/>
+      <c r="AX16" s="17"/>
+      <c r="AY16" s="17"/>
+      <c r="AZ16" s="17"/>
+      <c r="BA16" s="17"/>
+      <c r="BB16" s="17"/>
+      <c r="BC16" s="17"/>
+      <c r="BD16" s="17"/>
+      <c r="BE16" s="17"/>
+      <c r="BF16" s="17"/>
+      <c r="BG16" s="17"/>
+    </row>
+    <row r="17" spans="3:59" x14ac:dyDescent="0.45">
+      <c r="C17" t="s">
+        <v>385</v>
+      </c>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="15"/>
+      <c r="I17" s="14"/>
+      <c r="J17" s="14"/>
+      <c r="K17" s="14"/>
+      <c r="L17" s="14"/>
+      <c r="M17" s="14"/>
+      <c r="N17" s="14"/>
+      <c r="O17" s="14"/>
+      <c r="P17" s="14"/>
+      <c r="Q17" s="14"/>
+      <c r="R17" s="14"/>
+      <c r="S17" s="14"/>
+      <c r="T17" s="14"/>
+      <c r="U17" s="14"/>
+      <c r="V17" s="14"/>
+      <c r="W17" s="14"/>
+      <c r="X17" s="14"/>
+      <c r="Y17" s="14"/>
+      <c r="Z17" s="14"/>
+      <c r="AA17" s="14"/>
+      <c r="AB17" s="14"/>
+      <c r="AC17" s="14"/>
+      <c r="AD17" s="14"/>
+      <c r="AE17" s="14"/>
+      <c r="AF17" s="14"/>
+      <c r="AG17" s="14"/>
+      <c r="AH17" s="14"/>
+      <c r="AI17" s="14"/>
+      <c r="AJ17" s="14"/>
+      <c r="AK17" s="14"/>
+      <c r="AL17" s="14"/>
+      <c r="AM17" s="14"/>
+      <c r="AN17" s="14"/>
+      <c r="AO17" s="14"/>
+      <c r="AP17" s="14"/>
+      <c r="AQ17" s="14"/>
+      <c r="AR17" s="15"/>
+      <c r="AS17" s="15"/>
+      <c r="AT17" s="15"/>
+      <c r="AU17" s="15"/>
+      <c r="AV17" s="15"/>
+      <c r="AW17" s="15"/>
+      <c r="AX17" s="15"/>
+      <c r="AY17" s="15"/>
+      <c r="AZ17" s="15"/>
+      <c r="BA17" s="15"/>
+      <c r="BB17" s="15"/>
+      <c r="BC17" s="15"/>
+      <c r="BD17" s="15"/>
+      <c r="BE17" s="15"/>
+      <c r="BF17" s="15"/>
+      <c r="BG17" s="15"/>
+    </row>
+    <row r="18" spans="3:59" x14ac:dyDescent="0.45">
+      <c r="C18" t="s">
+        <v>386</v>
+      </c>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="15"/>
+      <c r="I18" s="15"/>
+      <c r="J18" s="15"/>
+      <c r="K18" s="15"/>
+      <c r="L18" s="15"/>
+      <c r="M18" s="15"/>
+      <c r="N18" s="15"/>
+      <c r="O18" s="15"/>
+      <c r="P18" s="15"/>
+      <c r="Q18" s="15"/>
+      <c r="R18" s="15"/>
+      <c r="S18" s="15"/>
+      <c r="T18" s="15"/>
+      <c r="U18" s="15"/>
+      <c r="V18" s="15"/>
+      <c r="W18" s="15"/>
+      <c r="X18" s="15"/>
+      <c r="Y18" s="15"/>
+      <c r="Z18" s="15"/>
+      <c r="AA18" s="15"/>
+      <c r="AB18" s="14"/>
+      <c r="AC18" s="15"/>
+      <c r="AD18" s="15"/>
+      <c r="AE18" s="15"/>
+      <c r="AF18" s="15"/>
+      <c r="AG18" s="15"/>
+      <c r="AH18" s="15"/>
+      <c r="AI18" s="15"/>
+      <c r="AJ18" s="15"/>
+      <c r="AK18" s="15"/>
+      <c r="AL18" s="15"/>
+      <c r="AM18" s="15"/>
+      <c r="AN18" s="15"/>
+      <c r="AO18" s="15"/>
+      <c r="AP18" s="15"/>
+      <c r="AQ18" s="15"/>
+      <c r="AR18" s="15"/>
+      <c r="AS18" s="15"/>
+      <c r="AT18" s="15"/>
+      <c r="AU18" s="15"/>
+      <c r="AV18" s="15"/>
+      <c r="AW18" s="15"/>
+      <c r="AX18" s="15"/>
+      <c r="AY18" s="15"/>
+      <c r="AZ18" s="15"/>
+      <c r="BA18" s="15"/>
+      <c r="BB18" s="15"/>
+      <c r="BC18" s="15"/>
+      <c r="BD18" s="15"/>
+      <c r="BE18" s="15"/>
+      <c r="BF18" s="15"/>
+      <c r="BG18" s="15"/>
+    </row>
+    <row r="19" spans="3:59" x14ac:dyDescent="0.45">
+      <c r="C19" t="s">
+        <v>387</v>
+      </c>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="15"/>
+      <c r="H19" s="15"/>
+      <c r="I19" s="15"/>
+      <c r="J19" s="15"/>
+      <c r="K19" s="15"/>
+      <c r="L19" s="15"/>
+      <c r="M19" s="15"/>
+      <c r="N19" s="15"/>
+      <c r="O19" s="15"/>
+      <c r="P19" s="15"/>
+      <c r="Q19" s="15"/>
+      <c r="R19" s="15"/>
+      <c r="S19" s="15"/>
+      <c r="T19" s="15"/>
+      <c r="U19" s="15"/>
+      <c r="V19" s="15"/>
+      <c r="W19" s="15"/>
+      <c r="X19" s="15"/>
+      <c r="Y19" s="15"/>
+      <c r="Z19" s="15"/>
+      <c r="AA19" s="15"/>
+      <c r="AB19" s="14"/>
+      <c r="AC19" s="15"/>
+      <c r="AD19" s="15"/>
+      <c r="AE19" s="15"/>
+      <c r="AF19" s="15"/>
+      <c r="AG19" s="15"/>
+      <c r="AH19" s="15"/>
+      <c r="AI19" s="15"/>
+      <c r="AJ19" s="15"/>
+      <c r="AK19" s="15"/>
+      <c r="AL19" s="15"/>
+      <c r="AM19" s="15"/>
+      <c r="AN19" s="15"/>
+      <c r="AO19" s="15"/>
+      <c r="AP19" s="15"/>
+      <c r="AQ19" s="15"/>
+      <c r="AR19" s="15"/>
+      <c r="AS19" s="15"/>
+      <c r="AT19" s="15"/>
+      <c r="AU19" s="15"/>
+      <c r="AV19" s="15"/>
+      <c r="AW19" s="15"/>
+      <c r="AX19" s="15"/>
+      <c r="AY19" s="15"/>
+      <c r="AZ19" s="15"/>
+      <c r="BA19" s="15"/>
+      <c r="BB19" s="15"/>
+      <c r="BC19" s="15"/>
+      <c r="BD19" s="15"/>
+      <c r="BE19" s="15"/>
+      <c r="BF19" s="15"/>
+      <c r="BG19" s="15"/>
+    </row>
+    <row r="20" spans="3:59" x14ac:dyDescent="0.45">
+      <c r="C20" t="s">
+        <v>388</v>
+      </c>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="15"/>
+      <c r="H20" s="15"/>
+      <c r="I20" s="15"/>
+      <c r="J20" s="15"/>
+      <c r="K20" s="15"/>
+      <c r="L20" s="15"/>
+      <c r="M20" s="15"/>
+      <c r="N20" s="15"/>
+      <c r="O20" s="15"/>
+      <c r="P20" s="15"/>
+      <c r="Q20" s="15"/>
+      <c r="R20" s="15"/>
+      <c r="S20" s="15"/>
+      <c r="T20" s="15"/>
+      <c r="U20" s="15"/>
+      <c r="V20" s="15"/>
+      <c r="W20" s="15"/>
+      <c r="X20" s="15"/>
+      <c r="Y20" s="15"/>
+      <c r="Z20" s="15"/>
+      <c r="AA20" s="15"/>
+      <c r="AB20" s="15"/>
+      <c r="AC20" s="14"/>
+      <c r="AD20" s="14"/>
+      <c r="AE20" s="15"/>
+      <c r="AF20" s="15"/>
+      <c r="AG20" s="15"/>
+      <c r="AH20" s="15"/>
+      <c r="AI20" s="15"/>
+      <c r="AJ20" s="15"/>
+      <c r="AK20" s="15"/>
+      <c r="AL20" s="15"/>
+      <c r="AM20" s="15"/>
+      <c r="AN20" s="15"/>
+      <c r="AO20" s="15"/>
+      <c r="AP20" s="15"/>
+      <c r="AQ20" s="15"/>
+      <c r="AR20" s="15"/>
+      <c r="AS20" s="15"/>
+      <c r="AT20" s="15"/>
+      <c r="AU20" s="15"/>
+      <c r="AV20" s="15"/>
+      <c r="AW20" s="15"/>
+      <c r="AX20" s="15"/>
+      <c r="AY20" s="15"/>
+      <c r="AZ20" s="15"/>
+      <c r="BA20" s="15"/>
+      <c r="BB20" s="15"/>
+      <c r="BC20" s="15"/>
+      <c r="BD20" s="15"/>
+      <c r="BE20" s="15"/>
+      <c r="BF20" s="15"/>
+      <c r="BG20" s="15"/>
+    </row>
+    <row r="21" spans="3:59" x14ac:dyDescent="0.45">
+      <c r="C21" t="s">
+        <v>389</v>
+      </c>
+      <c r="D21" s="15"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="15"/>
+      <c r="H21" s="15"/>
+      <c r="I21" s="15"/>
+      <c r="J21" s="15"/>
+      <c r="K21" s="15"/>
+      <c r="L21" s="15"/>
+      <c r="M21" s="15"/>
+      <c r="N21" s="15"/>
+      <c r="O21" s="15"/>
+      <c r="P21" s="15"/>
+      <c r="Q21" s="15"/>
+      <c r="R21" s="15"/>
+      <c r="S21" s="15"/>
+      <c r="T21" s="15"/>
+      <c r="U21" s="15"/>
+      <c r="V21" s="15"/>
+      <c r="W21" s="15"/>
+      <c r="X21" s="15"/>
+      <c r="Y21" s="15"/>
+      <c r="Z21" s="15"/>
+      <c r="AA21" s="15"/>
+      <c r="AB21" s="15"/>
+      <c r="AC21" s="14"/>
+      <c r="AD21" s="14"/>
+      <c r="AE21" s="14"/>
+      <c r="AF21" s="14"/>
+      <c r="AG21" s="14"/>
+      <c r="AH21" s="14"/>
+      <c r="AI21" s="14"/>
+      <c r="AJ21" s="14"/>
+      <c r="AK21" s="14"/>
+      <c r="AL21" s="14"/>
+      <c r="AM21" s="14"/>
+      <c r="AN21" s="14"/>
+      <c r="AO21" s="14"/>
+      <c r="AP21" s="14"/>
+      <c r="AQ21" s="14"/>
+      <c r="AR21" s="15"/>
+      <c r="AS21" s="15"/>
+      <c r="AT21" s="15"/>
+      <c r="AU21" s="15"/>
+      <c r="AV21" s="15"/>
+      <c r="AW21" s="15"/>
+      <c r="AX21" s="15"/>
+      <c r="AY21" s="15"/>
+      <c r="AZ21" s="15"/>
+      <c r="BA21" s="15"/>
+      <c r="BB21" s="15"/>
+      <c r="BC21" s="15"/>
+      <c r="BD21" s="15"/>
+      <c r="BE21" s="15"/>
+      <c r="BF21" s="15"/>
+      <c r="BG21" s="15"/>
+    </row>
+    <row r="22" spans="3:59" x14ac:dyDescent="0.45">
+      <c r="C22" t="s">
+        <v>390</v>
+      </c>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="15"/>
+      <c r="H22" s="15"/>
+      <c r="I22" s="15"/>
+      <c r="J22" s="15"/>
+      <c r="K22" s="15"/>
+      <c r="L22" s="15"/>
+      <c r="M22" s="15"/>
+      <c r="N22" s="15"/>
+      <c r="O22" s="15"/>
+      <c r="P22" s="15"/>
+      <c r="Q22" s="15"/>
+      <c r="R22" s="15"/>
+      <c r="S22" s="15"/>
+      <c r="T22" s="15"/>
+      <c r="U22" s="15"/>
+      <c r="V22" s="15"/>
+      <c r="W22" s="15"/>
+      <c r="X22" s="15"/>
+      <c r="Y22" s="15"/>
+      <c r="Z22" s="15"/>
+      <c r="AA22" s="15"/>
+      <c r="AB22" s="15"/>
+      <c r="AC22" s="15"/>
+      <c r="AD22" s="15"/>
+      <c r="AE22" s="15"/>
+      <c r="AF22" s="15"/>
+      <c r="AG22" s="15"/>
+      <c r="AH22" s="15"/>
+      <c r="AI22" s="15"/>
+      <c r="AJ22" s="15"/>
+      <c r="AK22" s="14"/>
+      <c r="AL22" s="14"/>
+      <c r="AM22" s="14"/>
+      <c r="AN22" s="14"/>
+      <c r="AO22" s="14"/>
+      <c r="AP22" s="14"/>
+      <c r="AQ22" s="14"/>
+      <c r="AR22" s="14"/>
+      <c r="AS22" s="14"/>
+      <c r="AT22" s="14"/>
+      <c r="AU22" s="14"/>
+      <c r="AV22" s="14"/>
+      <c r="AW22" s="14"/>
+      <c r="AX22" s="14"/>
+      <c r="AY22" s="14"/>
+      <c r="AZ22" s="14"/>
+      <c r="BA22" s="14"/>
+      <c r="BB22" s="14"/>
+      <c r="BC22" s="14"/>
+      <c r="BD22" s="15"/>
+      <c r="BE22" s="15"/>
+      <c r="BF22" s="15"/>
+      <c r="BG22" s="15"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
[5823 hvnl] Add scenario template to git
</commit_message>
<xml_diff>
--- a/historisch.xlsx
+++ b/historisch.xlsx
@@ -8,27 +8,29 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Code\quickdrive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF83839A-38D3-4105-ADB0-A7B6117CE3CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7893664C-E721-4ADE-9D5E-B96A64F723AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1365" yWindow="2138" windowWidth="15247" windowHeight="11647" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2040" yWindow="2813" windowWidth="15247" windowHeight="11647" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DRGLs" sheetId="10" r:id="rId1"/>
     <sheet name="76-77" sheetId="9" r:id="rId2"/>
     <sheet name="86-87" sheetId="1" r:id="rId3"/>
-    <sheet name="95-96" sheetId="2" r:id="rId4"/>
-    <sheet name="96-97" sheetId="3" r:id="rId5"/>
-    <sheet name="Goederenwagens" sheetId="6" r:id="rId6"/>
-    <sheet name="D-Treinen" sheetId="7" r:id="rId7"/>
-    <sheet name="Tijdlijn" sheetId="8" r:id="rId8"/>
+    <sheet name="88-89" sheetId="11" r:id="rId4"/>
+    <sheet name="95-96" sheetId="2" r:id="rId5"/>
+    <sheet name="96-97" sheetId="3" r:id="rId6"/>
+    <sheet name="Goederenwagens" sheetId="6" r:id="rId7"/>
+    <sheet name="D-Treinen" sheetId="7" r:id="rId8"/>
+    <sheet name="Tijdlijn" sheetId="8" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'76-77'!$A$1:$D$138</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'86-87'!$A$1:$D$115</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'95-96'!$A$1:$C$100</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'96-97'!$A$1:$C$99</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'D-Treinen'!$A$1:$H$562</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Goederenwagens!$A$1:$I$52</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'88-89'!$A$1:$F$120</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'95-96'!$A$1:$C$100</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'96-97'!$A$1:$C$99</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'D-Treinen'!$A$1:$H$562</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">Goederenwagens!$A$1:$I$52</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -45,7 +47,7 @@
     <author>Tom</author>
   </authors>
   <commentList>
-    <comment ref="A14" authorId="0" shapeId="0" xr:uid="{5646F17B-F3F5-4952-9E9F-2EEFBDD29067}">
+    <comment ref="H12" authorId="0" shapeId="0" xr:uid="{54C07705-8E2D-4609-86C5-050BA9493F35}">
       <text>
         <r>
           <rPr>
@@ -65,12 +67,11 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Nieuwere Plan E
-Rijtuigen aan Noordzijde</t>
+Geen 1600</t>
         </r>
       </text>
     </comment>
-    <comment ref="A21" authorId="0" shapeId="0" xr:uid="{3CB69F52-5C2D-47A9-A083-B96BB2EA83F5}">
+    <comment ref="N12" authorId="0" shapeId="0" xr:uid="{342D758B-A196-4440-97C0-83642F496C92}">
       <text>
         <r>
           <rPr>
@@ -90,12 +91,11 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Nieuwere Plan E
-Rijtuigen aan Noordzijde</t>
+Instroom ICR</t>
         </r>
       </text>
     </comment>
-    <comment ref="B33" authorId="0" shapeId="0" xr:uid="{61A0CC60-F010-45CF-933E-E1850291AC2D}">
+    <comment ref="B18" authorId="0" shapeId="0" xr:uid="{9056958B-79F5-4FFB-8ABE-AB9F33AB0691}">
       <text>
         <r>
           <rPr>
@@ -115,11 +115,11 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-1918</t>
+Schiphol westtak</t>
         </r>
       </text>
     </comment>
-    <comment ref="B46" authorId="0" shapeId="0" xr:uid="{42EFDC62-D205-4C5A-B710-AEB6F26A78C5}">
+    <comment ref="B20" authorId="0" shapeId="0" xr:uid="{7A8FE4D8-338B-4683-A70A-0C80047B1C26}">
       <text>
         <r>
           <rPr>
@@ -139,11 +139,11 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-2669</t>
+Bdpb</t>
         </r>
       </text>
     </comment>
-    <comment ref="B52" authorId="0" shapeId="0" xr:uid="{5EC7B95D-7C7E-4CD1-AAA9-1B61FAE6692C}">
+    <comment ref="O23" authorId="0" shapeId="0" xr:uid="{5FA3DDDE-9C2F-4197-B771-9705CB3B26FC}">
       <text>
         <r>
           <rPr>
@@ -163,11 +163,11 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-3363</t>
+M2</t>
         </r>
       </text>
     </comment>
-    <comment ref="B62" authorId="0" shapeId="0" xr:uid="{434D2A71-98D9-4E03-AAC9-6A74DEF0B234}">
+    <comment ref="AG23" authorId="0" shapeId="0" xr:uid="{95619DB4-C128-4B86-AB34-3E63E08EFD99}">
       <text>
         <r>
           <rPr>
@@ -187,13 +187,11 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-4714
-4716
-4765</t>
+Instroom DD-AR</t>
         </r>
       </text>
     </comment>
-    <comment ref="B67" authorId="0" shapeId="0" xr:uid="{1EBF6095-EC16-47D9-8BF4-CCD559BC4C0C}">
+    <comment ref="B28" authorId="0" shapeId="0" xr:uid="{D39C4451-48C2-450C-AF70-D2FC0941DDD1}">
       <text>
         <r>
           <rPr>
@@ -213,13 +211,11 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-5120
-5133
-5165</t>
+Thalys</t>
         </r>
       </text>
     </comment>
-    <comment ref="B69" authorId="0" shapeId="0" xr:uid="{6B104ADD-91D2-4EAA-98B2-84D5AD9AB1B4}">
+    <comment ref="F32" authorId="0" shapeId="0" xr:uid="{E8A63B2F-648A-463B-978E-2B922099EEB8}">
       <text>
         <r>
           <rPr>
@@ -239,12 +235,11 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-5418
-5463</t>
+Laatste jaar 1300 (P)</t>
         </r>
       </text>
     </comment>
-    <comment ref="A112" authorId="0" shapeId="0" xr:uid="{1FDA8098-BE5A-42E4-95D2-17545BCB68C3}">
+    <comment ref="O32" authorId="0" shapeId="0" xr:uid="{BB8FA2D5-D5DB-44F1-B6CD-E1E5297F36F1}">
       <text>
         <r>
           <rPr>
@@ -264,8 +259,103 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Nieuwere Plan E
-Rijtuigen aan Noordzijde</t>
+M2</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="P32" authorId="0" shapeId="0" xr:uid="{AF2D9712-3997-4646-A2F1-56004B710192}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Tom:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+K4</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B41" authorId="0" shapeId="0" xr:uid="{487BD35F-38A9-4E38-A4DF-64E8CE1CE3C9}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Tom:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+HSL Asd-Rtd</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="R41" authorId="0" shapeId="0" xr:uid="{4B88CDAC-D411-41FE-847D-CE08D2CA1DD5}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Tom:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+ICL</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="W41" authorId="0" shapeId="0" xr:uid="{F1D7DB00-E80A-43F1-9E85-E96D56FE2C2C}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Tom:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Laatste jaar Plan T</t>
         </r>
       </text>
     </comment>
@@ -279,7 +369,7 @@
     <author>Tom</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{1036B289-6974-449E-BE10-9F0D99FE17FE}">
+    <comment ref="A14" authorId="0" shapeId="0" xr:uid="{5646F17B-F3F5-4952-9E9F-2EEFBDD29067}">
       <text>
         <r>
           <rPr>
@@ -299,14 +389,12 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-https://www.youtube.com/watch?v=G2moQpXU-y4
-https://www.youtube.com/playlist?list=PLLWFxr62fBUn7FdsWCjL8tEsPKrSNfX6d
-https://www.youtube.com/playlist?list=PLvoHMQLV7GBS1DuSrTAnoqD6crT-Mv6Zi
-https://www.flickr.com/photos/bossie441/21515416066/</t>
+Nieuwere Plan E
+Rijtuigen aan Noordzijde</t>
         </r>
       </text>
     </comment>
-    <comment ref="F5" authorId="0" shapeId="0" xr:uid="{5E8B1808-5962-43EA-9A2C-AE75D3F8D3B7}">
+    <comment ref="A21" authorId="0" shapeId="0" xr:uid="{3CB69F52-5C2D-47A9-A083-B96BB2EA83F5}">
       <text>
         <r>
           <rPr>
@@ -326,11 +414,12 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-wel Klmos</t>
+Nieuwere Plan E
+Rijtuigen aan Noordzijde</t>
         </r>
       </text>
     </comment>
-    <comment ref="C7" authorId="0" shapeId="0" xr:uid="{B32A2D0B-0879-4A19-86A8-51F18C490063}">
+    <comment ref="B33" authorId="0" shapeId="0" xr:uid="{61A0CC60-F010-45CF-933E-E1850291AC2D}">
       <text>
         <r>
           <rPr>
@@ -350,11 +439,11 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-is CT GTOW/GTU?</t>
+1918</t>
         </r>
       </text>
     </comment>
-    <comment ref="F9" authorId="0" shapeId="0" xr:uid="{AF5FA88B-3737-40AA-BB50-FA1F52203947}">
+    <comment ref="B46" authorId="0" shapeId="0" xr:uid="{42EFDC62-D205-4C5A-B710-AEB6F26A78C5}">
       <text>
         <r>
           <rPr>
@@ -374,11 +463,11 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Alleen van WG, maar dan vind ik de Falns mooier</t>
+2669</t>
         </r>
       </text>
     </comment>
-    <comment ref="C11" authorId="0" shapeId="0" xr:uid="{B789BCCC-CD57-4B0F-BE83-94D2BA951D8E}">
+    <comment ref="B52" authorId="0" shapeId="0" xr:uid="{5EC7B95D-7C7E-4CD1-AAA9-1B61FAE6692C}">
       <text>
         <r>
           <rPr>
@@ -398,11 +487,11 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-langer dan Fccpps</t>
+3363</t>
         </r>
       </text>
     </comment>
-    <comment ref="F12" authorId="0" shapeId="0" xr:uid="{F5AC4812-E82A-4101-928B-04D2EDCE011B}">
+    <comment ref="B62" authorId="0" shapeId="0" xr:uid="{434D2A71-98D9-4E03-AAC9-6A74DEF0B234}">
       <text>
         <r>
           <rPr>
@@ -422,11 +511,13 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-lijkt op Fcs</t>
+4714
+4716
+4765</t>
         </r>
       </text>
     </comment>
-    <comment ref="C13" authorId="0" shapeId="0" xr:uid="{73047B42-0A17-4102-9489-FC04164A4A4F}">
+    <comment ref="B67" authorId="0" shapeId="0" xr:uid="{1EBF6095-EC16-47D9-8BF4-CCD559BC4C0C}">
       <text>
         <r>
           <rPr>
@@ -446,11 +537,13 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-trapje aan kopse kant</t>
+5120
+5133
+5165</t>
         </r>
       </text>
     </comment>
-    <comment ref="C14" authorId="0" shapeId="0" xr:uid="{9508F0A4-AD74-4D05-AF11-F05292070DEF}">
+    <comment ref="B69" authorId="0" shapeId="0" xr:uid="{6B104ADD-91D2-4EAA-98B2-84D5AD9AB1B4}">
       <text>
         <r>
           <rPr>
@@ -470,11 +563,12 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-2 secties tussen luikjes</t>
+5418
+5463</t>
         </r>
       </text>
     </comment>
-    <comment ref="F14" authorId="0" shapeId="0" xr:uid="{23C4FBE5-3CB2-4D3E-9242-7CA96139C4AB}">
+    <comment ref="A112" authorId="0" shapeId="0" xr:uid="{1FDA8098-BE5A-42E4-95D2-17545BCB68C3}">
       <text>
         <r>
           <rPr>
@@ -494,367 +588,8 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Evt ChrisTrains</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C15" authorId="0" shapeId="0" xr:uid="{A5791D67-C441-4DA9-9E08-03BD7F6C47E1}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Tom:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-2 luikjes, schuifdeur</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C16" authorId="0" shapeId="0" xr:uid="{E9476943-4328-4D1E-B102-F21B1F084DA5}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Tom:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-1 sectie tussen luikjes</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F20" authorId="0" shapeId="0" xr:uid="{1ADEB68A-8A9E-4978-AD89-4DFF9A1AFFD5}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Tom:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Evt ChrisTrains</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F24" authorId="0" shapeId="0" xr:uid="{F8AE0030-48E1-4B2E-9A56-09A764892F91}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Tom:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-wel Klmos</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F29" authorId="0" shapeId="0" xr:uid="{C20E7EC7-D934-4AEA-8C93-D2017EBF9531}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Tom:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-3dz statisch beladen maar allen rood :/</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F32" authorId="0" shapeId="0" xr:uid="{24FC3703-310F-4862-B9DC-25D6B9DC8193}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Tom:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-wel Slmmnps</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C33" authorId="0" shapeId="0" xr:uid="{C3553452-DD50-4222-BBA4-FA91EF233F0F}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Tom:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-verdiept</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F33" authorId="0" shapeId="0" xr:uid="{61DE6817-D051-403A-A70C-9E7DC23A6DD8}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Tom:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-wel Slmmnps</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C34" authorId="0" shapeId="0" xr:uid="{792E746E-F741-477D-9465-6A06CD44BF02}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Tom:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-plat</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F34" authorId="0" shapeId="0" xr:uid="{7E233B53-B1EA-4730-A7DD-B7755BA09966}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Tom:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-wel Slmmnps</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C35" authorId="0" shapeId="0" xr:uid="{7B5D9B84-4DD8-401B-A35B-3951F8DAF1EC}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Tom:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-plat</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F35" authorId="0" shapeId="0" xr:uid="{C844A891-91A2-420C-99F4-1E4C68BF7B84}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Tom:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-wel Slmmnps</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C36" authorId="0" shapeId="0" xr:uid="{73CCEB3B-4103-42AA-A8D9-1A70E78A5F9A}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Tom:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Volgens foto's, ipv Tads</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C46" authorId="0" shapeId="0" xr:uid="{1AE6750D-EEF2-4B34-A9F8-451E2329DE11}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Tom:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-is Klmos?</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C48" authorId="0" shapeId="0" xr:uid="{E7905AA8-B65B-413C-A73A-1C1AD6BEEFB8}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Tom:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Bordes bovenop tot halverwege</t>
+Nieuwere Plan E
+Rijtuigen aan Noordzijde</t>
         </r>
       </text>
     </comment>
@@ -868,6 +603,595 @@
     <author>Tom</author>
   </authors>
   <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{1036B289-6974-449E-BE10-9F0D99FE17FE}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Tom:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+https://www.youtube.com/watch?v=G2moQpXU-y4
+https://www.youtube.com/playlist?list=PLLWFxr62fBUn7FdsWCjL8tEsPKrSNfX6d
+https://www.youtube.com/playlist?list=PLvoHMQLV7GBS1DuSrTAnoqD6crT-Mv6Zi
+https://www.flickr.com/photos/bossie441/21515416066/</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F5" authorId="0" shapeId="0" xr:uid="{5E8B1808-5962-43EA-9A2C-AE75D3F8D3B7}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Tom:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+wel Klmos</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C7" authorId="0" shapeId="0" xr:uid="{B32A2D0B-0879-4A19-86A8-51F18C490063}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Tom:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+is CT GTOW/GTU?</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F9" authorId="0" shapeId="0" xr:uid="{AF5FA88B-3737-40AA-BB50-FA1F52203947}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Tom:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Alleen van WG, maar dan vind ik de Falns mooier</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C11" authorId="0" shapeId="0" xr:uid="{B789BCCC-CD57-4B0F-BE83-94D2BA951D8E}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Tom:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+langer dan Fccpps</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F12" authorId="0" shapeId="0" xr:uid="{F5AC4812-E82A-4101-928B-04D2EDCE011B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Tom:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+lijkt op Fcs</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C13" authorId="0" shapeId="0" xr:uid="{73047B42-0A17-4102-9489-FC04164A4A4F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Tom:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+trapje aan kopse kant</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C14" authorId="0" shapeId="0" xr:uid="{9508F0A4-AD74-4D05-AF11-F05292070DEF}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Tom:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+2 secties tussen luikjes</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F14" authorId="0" shapeId="0" xr:uid="{23C4FBE5-3CB2-4D3E-9242-7CA96139C4AB}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Tom:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Evt ChrisTrains</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C15" authorId="0" shapeId="0" xr:uid="{A5791D67-C441-4DA9-9E08-03BD7F6C47E1}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Tom:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+2 luikjes, schuifdeur</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C16" authorId="0" shapeId="0" xr:uid="{E9476943-4328-4D1E-B102-F21B1F084DA5}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Tom:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+1 sectie tussen luikjes</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F20" authorId="0" shapeId="0" xr:uid="{1ADEB68A-8A9E-4978-AD89-4DFF9A1AFFD5}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Tom:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Evt ChrisTrains</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F24" authorId="0" shapeId="0" xr:uid="{F8AE0030-48E1-4B2E-9A56-09A764892F91}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Tom:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+wel Klmos</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F29" authorId="0" shapeId="0" xr:uid="{C20E7EC7-D934-4AEA-8C93-D2017EBF9531}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Tom:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+3dz statisch beladen maar allen rood :/</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F32" authorId="0" shapeId="0" xr:uid="{24FC3703-310F-4862-B9DC-25D6B9DC8193}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Tom:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+wel Slmmnps</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C33" authorId="0" shapeId="0" xr:uid="{C3553452-DD50-4222-BBA4-FA91EF233F0F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Tom:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+verdiept</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F33" authorId="0" shapeId="0" xr:uid="{61DE6817-D051-403A-A70C-9E7DC23A6DD8}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Tom:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+wel Slmmnps</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C34" authorId="0" shapeId="0" xr:uid="{792E746E-F741-477D-9465-6A06CD44BF02}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Tom:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+plat</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F34" authorId="0" shapeId="0" xr:uid="{7E233B53-B1EA-4730-A7DD-B7755BA09966}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Tom:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+wel Slmmnps</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C35" authorId="0" shapeId="0" xr:uid="{7B5D9B84-4DD8-401B-A35B-3951F8DAF1EC}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Tom:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+plat</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F35" authorId="0" shapeId="0" xr:uid="{C844A891-91A2-420C-99F4-1E4C68BF7B84}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Tom:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+wel Slmmnps</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C36" authorId="0" shapeId="0" xr:uid="{73CCEB3B-4103-42AA-A8D9-1A70E78A5F9A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Tom:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Volgens foto's, ipv Tads</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C46" authorId="0" shapeId="0" xr:uid="{1AE6750D-EEF2-4B34-A9F8-451E2329DE11}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Tom:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+is Klmos?</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C48" authorId="0" shapeId="0" xr:uid="{E7905AA8-B65B-413C-A73A-1C1AD6BEEFB8}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Tom:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Bordes bovenop tot halverwege</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Tom</author>
+  </authors>
+  <commentList>
     <comment ref="G1" authorId="0" shapeId="0" xr:uid="{10DC490D-CF53-453A-906C-1C94B8CA3BEB}">
       <text>
         <r>
@@ -4715,7 +5039,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3545" uniqueCount="487">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3643" uniqueCount="501">
   <si>
     <t>ICM (KLM, Martinair)</t>
   </si>
@@ -6327,6 +6651,48 @@
       </rPr>
       <t>; Sluiting IJmuiden</t>
     </r>
+  </si>
+  <si>
+    <t>Serie</t>
+  </si>
+  <si>
+    <t>Route</t>
+  </si>
+  <si>
+    <t>Es-Rtd/Gvc</t>
+  </si>
+  <si>
+    <t>IC</t>
+  </si>
+  <si>
+    <t>St</t>
+  </si>
+  <si>
+    <t>Gvc-Ut</t>
+  </si>
+  <si>
+    <t>Rtd-Gd</t>
+  </si>
+  <si>
+    <t>Gd-Apn</t>
+  </si>
+  <si>
+    <t>Rtd-Gd-Asd</t>
+  </si>
+  <si>
+    <t>Rtd/Gvc-Ah-Zp</t>
+  </si>
+  <si>
+    <t>Ut-Ledn</t>
+  </si>
+  <si>
+    <t>TS - GH</t>
+  </si>
+  <si>
+    <t>Ut-Ehv?</t>
+  </si>
+  <si>
+    <t>Gn/Lw-Rtd-Gvc</t>
   </si>
 </sst>
 </file>
@@ -6450,7 +6816,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -6508,6 +6874,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -6789,14 +7158,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{489B176B-B4D8-4CE5-87AC-D8FCFCF601A3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{489B176B-B4D8-4CE5-87AC-D8FCFCF601A3}">
   <dimension ref="A1:AJ54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AJ16" sqref="AJ16"/>
+      <selection pane="bottomRight" activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -9946,6 +10315,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -12308,6 +12678,927 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72466DAB-8B29-4FEF-B82D-F42B6950440C}">
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:F120"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="9.1328125" customWidth="1"/>
+    <col min="3" max="3" width="19.265625" customWidth="1"/>
+    <col min="4" max="4" width="18.6640625" customWidth="1"/>
+    <col min="6" max="6" width="2.59765625" style="21" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="36.4" x14ac:dyDescent="0.45">
+      <c r="A1" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>487</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>488</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="F1" s="26" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="B3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="B4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="B5">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="B6">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="B7">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="B8">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="B9">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="B10">
+        <v>500</v>
+      </c>
+      <c r="C10" t="s">
+        <v>400</v>
+      </c>
+      <c r="D10" t="s">
+        <v>500</v>
+      </c>
+      <c r="F10" s="21" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="B11">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="B12">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="B13">
+        <v>700</v>
+      </c>
+      <c r="C13" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="B14">
+        <v>800</v>
+      </c>
+      <c r="C14" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="B15">
+        <v>800</v>
+      </c>
+      <c r="C15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="B16">
+        <v>800</v>
+      </c>
+      <c r="C16" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="B17">
+        <v>800</v>
+      </c>
+      <c r="C17" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="B18">
+        <v>900</v>
+      </c>
+      <c r="C18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="B19">
+        <v>900</v>
+      </c>
+      <c r="C19" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="B20">
+        <v>900</v>
+      </c>
+      <c r="C20" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="B21">
+        <v>1240</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="B22">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="B23">
+        <v>1600</v>
+      </c>
+      <c r="C23" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="B24">
+        <v>1600</v>
+      </c>
+      <c r="C24" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="B25">
+        <v>1600</v>
+      </c>
+      <c r="C25" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="B26">
+        <v>1600</v>
+      </c>
+      <c r="C26" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A27" t="s">
+        <v>490</v>
+      </c>
+      <c r="B27">
+        <v>1700</v>
+      </c>
+      <c r="C27" t="s">
+        <v>106</v>
+      </c>
+      <c r="D27" t="s">
+        <v>489</v>
+      </c>
+      <c r="F27" s="21" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A28" t="s">
+        <v>490</v>
+      </c>
+      <c r="B28">
+        <v>1700</v>
+      </c>
+      <c r="C28" t="s">
+        <v>400</v>
+      </c>
+      <c r="D28" t="s">
+        <v>489</v>
+      </c>
+      <c r="F28" s="21" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="B29">
+        <v>1800</v>
+      </c>
+      <c r="C29" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="B30">
+        <v>1900</v>
+      </c>
+      <c r="C30" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="B31">
+        <v>1900</v>
+      </c>
+      <c r="C31" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="B32">
+        <v>1900</v>
+      </c>
+      <c r="C32" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="B33">
+        <v>2100</v>
+      </c>
+      <c r="C33" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="B34">
+        <v>2100</v>
+      </c>
+      <c r="C34" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="B35">
+        <v>2240</v>
+      </c>
+      <c r="C35" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="B36">
+        <v>2300</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="B37">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="B38">
+        <v>2600</v>
+      </c>
+      <c r="C38" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="B39">
+        <v>2700</v>
+      </c>
+      <c r="C39" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="B40">
+        <v>2900</v>
+      </c>
+      <c r="C40" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="B41">
+        <v>3100</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="B42">
+        <v>3300</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A43" t="s">
+        <v>491</v>
+      </c>
+      <c r="B43">
+        <v>3500</v>
+      </c>
+      <c r="D43" t="s">
+        <v>494</v>
+      </c>
+      <c r="F43" s="21" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="B44">
+        <v>3600</v>
+      </c>
+      <c r="C44" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="B45">
+        <v>3730</v>
+      </c>
+      <c r="C45" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="B46">
+        <v>3760</v>
+      </c>
+      <c r="C46" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="B47">
+        <v>3780</v>
+      </c>
+      <c r="C47" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="B48">
+        <v>3900</v>
+      </c>
+      <c r="C48" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A49" t="s">
+        <v>491</v>
+      </c>
+      <c r="B49">
+        <v>4000</v>
+      </c>
+      <c r="C49" t="s">
+        <v>11</v>
+      </c>
+      <c r="D49" t="s">
+        <v>495</v>
+      </c>
+      <c r="F49" s="21" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="B50">
+        <v>4100</v>
+      </c>
+      <c r="C50" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="B51">
+        <v>4200</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="B52">
+        <v>4300</v>
+      </c>
+      <c r="C52" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="B53">
+        <v>4300</v>
+      </c>
+      <c r="C53" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="B54">
+        <v>4400</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="B55">
+        <v>4500</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="B56">
+        <v>4600</v>
+      </c>
+      <c r="C56" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="B57">
+        <v>4700</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="B58">
+        <v>4800</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="B59">
+        <v>4900</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="B60">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="B61">
+        <v>5100</v>
+      </c>
+      <c r="C61" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="B62">
+        <v>5200</v>
+      </c>
+      <c r="C62" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="B63">
+        <v>5300</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="B64">
+        <v>5400</v>
+      </c>
+      <c r="C64" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="65" spans="2:3" hidden="1" x14ac:dyDescent="0.45">
+      <c r="B65">
+        <v>5500</v>
+      </c>
+    </row>
+    <row r="66" spans="2:3" hidden="1" x14ac:dyDescent="0.45">
+      <c r="B66">
+        <v>5600</v>
+      </c>
+    </row>
+    <row r="67" spans="2:3" hidden="1" x14ac:dyDescent="0.45">
+      <c r="B67">
+        <v>5700</v>
+      </c>
+    </row>
+    <row r="68" spans="2:3" hidden="1" x14ac:dyDescent="0.45">
+      <c r="B68">
+        <v>5800</v>
+      </c>
+      <c r="C68" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="69" spans="2:3" hidden="1" x14ac:dyDescent="0.45">
+      <c r="B69">
+        <v>5900</v>
+      </c>
+    </row>
+    <row r="70" spans="2:3" hidden="1" x14ac:dyDescent="0.45">
+      <c r="B70">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="71" spans="2:3" hidden="1" x14ac:dyDescent="0.45">
+      <c r="B71">
+        <v>6100</v>
+      </c>
+      <c r="C71" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="72" spans="2:3" hidden="1" x14ac:dyDescent="0.45">
+      <c r="B72">
+        <v>6200</v>
+      </c>
+      <c r="C72" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="73" spans="2:3" hidden="1" x14ac:dyDescent="0.45">
+      <c r="B73">
+        <v>6300</v>
+      </c>
+    </row>
+    <row r="74" spans="2:3" hidden="1" x14ac:dyDescent="0.45">
+      <c r="B74">
+        <v>6400</v>
+      </c>
+    </row>
+    <row r="75" spans="2:3" hidden="1" x14ac:dyDescent="0.45">
+      <c r="B75">
+        <v>6500</v>
+      </c>
+      <c r="C75" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="76" spans="2:3" hidden="1" x14ac:dyDescent="0.45">
+      <c r="B76">
+        <v>6600</v>
+      </c>
+    </row>
+    <row r="77" spans="2:3" hidden="1" x14ac:dyDescent="0.45">
+      <c r="B77">
+        <v>6700</v>
+      </c>
+    </row>
+    <row r="78" spans="2:3" hidden="1" x14ac:dyDescent="0.45">
+      <c r="B78">
+        <v>6800</v>
+      </c>
+    </row>
+    <row r="79" spans="2:3" hidden="1" x14ac:dyDescent="0.45">
+      <c r="B79">
+        <v>6900</v>
+      </c>
+    </row>
+    <row r="80" spans="2:3" hidden="1" x14ac:dyDescent="0.45">
+      <c r="B80">
+        <v>7000</v>
+      </c>
+      <c r="C80" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="81" spans="2:3" hidden="1" x14ac:dyDescent="0.45">
+      <c r="B81">
+        <v>7000</v>
+      </c>
+      <c r="C81" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="82" spans="2:3" hidden="1" x14ac:dyDescent="0.45">
+      <c r="B82">
+        <v>7100</v>
+      </c>
+      <c r="C82" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="83" spans="2:3" hidden="1" x14ac:dyDescent="0.45">
+      <c r="B83">
+        <v>7200</v>
+      </c>
+    </row>
+    <row r="84" spans="2:3" hidden="1" x14ac:dyDescent="0.45">
+      <c r="B84">
+        <v>7300</v>
+      </c>
+      <c r="C84" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="85" spans="2:3" hidden="1" x14ac:dyDescent="0.45">
+      <c r="B85">
+        <v>7400</v>
+      </c>
+    </row>
+    <row r="86" spans="2:3" hidden="1" x14ac:dyDescent="0.45">
+      <c r="B86">
+        <v>7500</v>
+      </c>
+      <c r="C86" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="87" spans="2:3" hidden="1" x14ac:dyDescent="0.45">
+      <c r="B87">
+        <v>7600</v>
+      </c>
+    </row>
+    <row r="88" spans="2:3" hidden="1" x14ac:dyDescent="0.45">
+      <c r="B88">
+        <v>7700</v>
+      </c>
+      <c r="C88" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="89" spans="2:3" hidden="1" x14ac:dyDescent="0.45">
+      <c r="B89">
+        <v>7800</v>
+      </c>
+      <c r="C89" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="90" spans="2:3" hidden="1" x14ac:dyDescent="0.45">
+      <c r="B90">
+        <v>7900</v>
+      </c>
+    </row>
+    <row r="91" spans="2:3" hidden="1" x14ac:dyDescent="0.45">
+      <c r="B91">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="92" spans="2:3" hidden="1" x14ac:dyDescent="0.45">
+      <c r="B92">
+        <v>8100</v>
+      </c>
+      <c r="C92" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="93" spans="2:3" hidden="1" x14ac:dyDescent="0.45">
+      <c r="B93">
+        <v>8200</v>
+      </c>
+      <c r="C93" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="94" spans="2:3" hidden="1" x14ac:dyDescent="0.45">
+      <c r="B94">
+        <v>8300</v>
+      </c>
+      <c r="C94" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="95" spans="2:3" hidden="1" x14ac:dyDescent="0.45">
+      <c r="B95">
+        <v>8400</v>
+      </c>
+      <c r="C95" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="96" spans="2:3" hidden="1" x14ac:dyDescent="0.45">
+      <c r="B96">
+        <v>8500</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="B97">
+        <v>8600</v>
+      </c>
+      <c r="C97" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="B98">
+        <v>8700</v>
+      </c>
+      <c r="C98" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="B99">
+        <v>8800</v>
+      </c>
+      <c r="C99" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="B100">
+        <v>8900</v>
+      </c>
+      <c r="C100" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A101" t="s">
+        <v>491</v>
+      </c>
+      <c r="B101">
+        <v>9600</v>
+      </c>
+      <c r="C101" t="s">
+        <v>11</v>
+      </c>
+      <c r="D101" t="s">
+        <v>499</v>
+      </c>
+      <c r="F101" s="21" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="B102">
+        <v>9700</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A103" t="s">
+        <v>491</v>
+      </c>
+      <c r="B103">
+        <v>9800</v>
+      </c>
+      <c r="C103" t="s">
+        <v>11</v>
+      </c>
+      <c r="D103" t="s">
+        <v>496</v>
+      </c>
+      <c r="F103" s="21" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A104" t="s">
+        <v>491</v>
+      </c>
+      <c r="B104">
+        <v>9900</v>
+      </c>
+      <c r="D104" t="s">
+        <v>497</v>
+      </c>
+      <c r="F104" s="21" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="B105">
+        <v>13700</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="B106">
+        <v>14500</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="B107">
+        <v>14600</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="B108">
+        <v>14700</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="B109">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="B110">
+        <v>15200</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="B111">
+        <v>15600</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="B112">
+        <v>16800</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="B113">
+        <v>16900</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="B114">
+        <v>17700</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="B115">
+        <v>17800</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="B116">
+        <v>18800</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A117" t="s">
+        <v>491</v>
+      </c>
+      <c r="B117">
+        <v>19000</v>
+      </c>
+      <c r="D117" t="s">
+        <v>492</v>
+      </c>
+      <c r="F117" s="21" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A118" t="s">
+        <v>491</v>
+      </c>
+      <c r="B118">
+        <v>19300</v>
+      </c>
+      <c r="D118" t="s">
+        <v>493</v>
+      </c>
+      <c r="F118" s="21" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A119" t="s">
+        <v>491</v>
+      </c>
+      <c r="B119">
+        <v>19900</v>
+      </c>
+      <c r="C119" t="s">
+        <v>11</v>
+      </c>
+      <c r="D119" t="s">
+        <v>497</v>
+      </c>
+      <c r="F119" s="21" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="B120">
+        <v>31800</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:F120" xr:uid="{72466DAB-8B29-4FEF-B82D-F42B6950440C}">
+    <filterColumn colId="5">
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
+    </filterColumn>
+  </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0211A2A-DC69-448E-B36B-BE6820863E81}">
   <dimension ref="A1:C100"/>
   <sheetViews>
@@ -13373,7 +14664,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{778DD009-53DD-426B-BBA7-ABCE73A49F39}">
   <dimension ref="A1:C106"/>
   <sheetViews>
@@ -14261,7 +15552,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{379E3CDC-714A-4865-8067-4D8FDE224D87}">
   <dimension ref="A1:I52"/>
   <sheetViews>
@@ -15125,7 +16416,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DB840A4-93DF-43F4-B9FF-1DFD0858F8C3}">
   <dimension ref="A1:H417"/>
   <sheetViews>
@@ -24039,7 +25330,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5776901-1A98-4DFB-9BF8-9460FA86F060}">
   <dimension ref="A1:BG22"/>
   <sheetViews>

</xml_diff>

<commit_message>
WIP consists andere jaartallen
</commit_message>
<xml_diff>
--- a/historisch.xlsx
+++ b/historisch.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Code\quickdrive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69672508-5269-4315-8EE6-DFC5596E1EC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68CA6697-8AD3-4894-BD3F-ECA56F671ED0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DRGLs" sheetId="10" r:id="rId1"/>
@@ -775,6 +775,30 @@
         </r>
       </text>
     </comment>
+    <comment ref="F31" authorId="0" shapeId="0" xr:uid="{EA46AFE5-F982-4C64-BD2F-F2F559C510ED}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Tom:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Laatste jaar 1300</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="AB31" authorId="0" shapeId="0" xr:uid="{21D2FBFB-1C9F-4432-A836-1FB5D60141BD}">
       <text>
         <r>
@@ -824,30 +848,6 @@
 ACTS 1200
 Ludmilla
 M2, K4</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F32" authorId="0" shapeId="0" xr:uid="{E8A63B2F-648A-463B-978E-2B922099EEB8}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Tom:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Laatste jaar 1300 (P)</t>
         </r>
       </text>
     </comment>
@@ -6723,7 +6723,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3665" uniqueCount="504">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3664" uniqueCount="504">
   <si>
     <t>ICM (KLM, Martinair)</t>
   </si>
@@ -8890,10 +8890,10 @@
   <dimension ref="A1:AL54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C23" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F35" sqref="F35"/>
+      <selection pane="bottomRight" activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -11011,9 +11011,7 @@
       <c r="E32" s="22" t="s">
         <v>501</v>
       </c>
-      <c r="F32" s="22" t="s">
-        <v>456</v>
-      </c>
+      <c r="F32" s="22"/>
       <c r="G32" s="23"/>
       <c r="H32" s="22" t="s">
         <v>456</v>

</xml_diff>